<commit_message>
Se revision de la tarea
</commit_message>
<xml_diff>
--- a/Excel/Clase del 30 de Mayo.xlsx
+++ b/Excel/Clase del 30 de Mayo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clases-octave\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB41AEEC-C7D1-48F1-BD70-79108407D4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A5F87E-F890-44B9-8406-B5CCB7DF24C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{03D619B0-3462-4495-8F85-31A3C38CF12B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{03D619B0-3462-4495-8F85-31A3C38CF12B}"/>
   </bookViews>
   <sheets>
     <sheet name="Simpson 1l3" sheetId="1" r:id="rId1"/>
@@ -20016,11 +20016,11 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>725880</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId99">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="294" name="Entrada de lápiz 293">
@@ -20035,11 +20035,11 @@
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
             <a:off x="2179080" y="5996520"/>
-            <a:ext cx="2509200" cy="1298160"/>
+            <a:ext cx="2509200" cy="991080"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="294" name="Entrada de lápiz 293">
@@ -20059,8 +20059,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2161080" y="5978875"/>
-              <a:ext cx="2544840" cy="1333810"/>
+              <a:off x="2161080" y="5978520"/>
+              <a:ext cx="2544840" cy="1026720"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -20080,12 +20080,12 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>404880</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
+      <xdr:colOff>404520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>122040</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId101">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="307" name="Entrada de lápiz 306">
@@ -20100,11 +20100,11 @@
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
             <a:off x="4990680" y="6057360"/>
-            <a:ext cx="961560" cy="871560"/>
+            <a:ext cx="961200" cy="648360"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="307" name="Entrada de lápiz 306">
@@ -20124,8 +20124,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4972680" y="6039720"/>
-              <a:ext cx="997200" cy="907200"/>
+              <a:off x="4972680" y="6039360"/>
+              <a:ext cx="996840" cy="684000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -20659,201 +20659,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>570240</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>307200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId119">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="364" name="Entrada de lápiz 363">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAFF19DF-C0FC-4104-931A-F1DDE53E83AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7702560" y="6161040"/>
-            <a:ext cx="1321920" cy="312840"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="364" name="Entrada de lápiz 363">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAFF19DF-C0FC-4104-931A-F1DDE53E83AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId120"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7684565" y="6143019"/>
-              <a:ext cx="1357550" cy="348521"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>693120</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571680</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId121">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="375" name="Entrada de lápiz 374">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B8FDFF-A347-44DB-A046-2AC5EF1CBC2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="9410400" y="6012360"/>
-            <a:ext cx="671040" cy="436320"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="375" name="Entrada de lápiz 374">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B8FDFF-A347-44DB-A046-2AC5EF1CBC2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId122"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9392400" y="5994375"/>
-              <a:ext cx="706680" cy="471931"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584280</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>678240</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId123">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="376" name="Entrada de lápiz 375">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F87080-777C-41E4-8ECE-AF97B99B0DB3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="7716600" y="6202440"/>
-            <a:ext cx="93960" cy="14040"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="376" name="Entrada de lápiz 375">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F87080-777C-41E4-8ECE-AF97B99B0DB3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId124"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7698600" y="6184440"/>
-              <a:ext cx="129600" cy="49680"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>52920</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>98640</xdr:rowOff>
@@ -20866,7 +20671,7 @@
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId125">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId119">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="388" name="Entrada de lápiz 387">
               <a:extLst>
@@ -20918,201 +20723,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>288300</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>133620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>25260</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>80700</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId127">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="391" name="Entrada de lápiz 390">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C2FDC3-37B5-419A-BAD4-F25C27164168}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="8213100" y="7814580"/>
-            <a:ext cx="1321920" cy="312840"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="391" name="Entrada de lápiz 390">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C2FDC3-37B5-419A-BAD4-F25C27164168}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId120"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8195105" y="7796559"/>
-              <a:ext cx="1357550" cy="348521"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>98760</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>137340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>769800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>25020</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId128">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="392" name="Entrada de lápiz 391">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{287F2E2F-3F6C-46EB-A67E-55F5C181799A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="9608520" y="7635420"/>
-            <a:ext cx="671040" cy="436320"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="392" name="Entrada de lápiz 391">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{287F2E2F-3F6C-46EB-A67E-55F5C181799A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId122"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="9590520" y="7617435"/>
-              <a:ext cx="706680" cy="471931"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>302340</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>175020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>396300</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>6180</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId129">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="393" name="Entrada de lápiz 392">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E86131-D0D1-498B-9791-9D3C85E66026}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="8227140" y="7855980"/>
-            <a:ext cx="93960" cy="14040"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="393" name="Entrada de lápiz 392">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E86131-D0D1-498B-9791-9D3C85E66026}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId124"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8209140" y="7837980"/>
-              <a:ext cx="129600" cy="49680"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>60360</xdr:colOff>
       <xdr:row>41</xdr:row>
@@ -21126,7 +20736,7 @@
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId130">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId127">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="396" name="Entrada de lápiz 395">
               <a:extLst>
@@ -21185,12 +20795,12 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>15360</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId132">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="442" name="Entrada de lápiz 441">
@@ -21205,11 +20815,11 @@
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
             <a:off x="10840680" y="7310880"/>
-            <a:ext cx="5816760" cy="1017720"/>
+            <a:ext cx="5817240" cy="1017720"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="442" name="Entrada de lápiz 441">
@@ -21229,8 +20839,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10822680" y="7293240"/>
-              <a:ext cx="5852399" cy="1053360"/>
+              <a:off x="10822680" y="7292880"/>
+              <a:ext cx="5852880" cy="1053360"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -22414,24 +22024,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:colOff>250920</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>167100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>236280</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
+      <xdr:rowOff>129240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>472320</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId167">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="558" name="Entrada de lápiz 557">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27BC26-4881-498D-BC79-34F874DCA2AA}"/>
+            <xdr14:cNvPr id="32" name="Entrada de lápiz 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE84194E-5499-41CD-AB26-55EE26E71DD2}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -22439,18 +22049,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="16733520" y="6019260"/>
-            <a:ext cx="1729800" cy="739740"/>
+            <a:off x="16893000" y="5981400"/>
+            <a:ext cx="2598840" cy="830880"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="558" name="Entrada de lápiz 557">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F27BC26-4881-498D-BC79-34F874DCA2AA}"/>
+            <xdr:cNvPr id="32" name="Entrada de lápiz 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE84194E-5499-41CD-AB26-55EE26E71DD2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -22464,8 +22074,658 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="16715520" y="6001621"/>
-              <a:ext cx="1765440" cy="775377"/>
+              <a:off x="16875360" y="5963760"/>
+              <a:ext cx="2634480" cy="866520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>32520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>337800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId169">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="33" name="Entrada de lápiz 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB05AA2E-211D-4F8C-B77C-4F3DBB1D6AC4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2409960" y="6742080"/>
+            <a:ext cx="305280" cy="285480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="33" name="Entrada de lápiz 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB05AA2E-211D-4F8C-B77C-4F3DBB1D6AC4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId170"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2392320" y="6724440"/>
+              <a:ext cx="340920" cy="321120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>83040</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>83520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>618360</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId171">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="42" name="Entrada de lápiz 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D904351-644C-4383-9F46-7062D2F9AE83}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1668000" y="2826720"/>
+            <a:ext cx="535320" cy="295200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="42" name="Entrada de lápiz 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D904351-644C-4383-9F46-7062D2F9AE83}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId172"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1650012" y="2809080"/>
+              <a:ext cx="570936" cy="330840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>324600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489120</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>176400</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId173">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="43" name="Entrada de lápiz 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{489AD390-91ED-4AC1-BE4A-8A4460C6527B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4287000" y="7093080"/>
+            <a:ext cx="164520" cy="215640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="43" name="Entrada de lápiz 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{489AD390-91ED-4AC1-BE4A-8A4460C6527B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId174"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4269000" y="7075080"/>
+              <a:ext cx="200160" cy="251280"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>138240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335520</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId175">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="46" name="Entrada de lápiz 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA0D3D00-8AA4-4073-B969-3DC945F85659}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="5630880" y="6721920"/>
+            <a:ext cx="252000" cy="302040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="46" name="Entrada de lápiz 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA0D3D00-8AA4-4073-B969-3DC945F85659}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId176"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5612880" y="6704280"/>
+              <a:ext cx="287640" cy="337680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>624360</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>174960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>734520</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId177">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Entrada de lápiz 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333D9316-CD87-4239-846A-F72DCE9FE053}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7756680" y="6210000"/>
+            <a:ext cx="110160" cy="267120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="50" name="Entrada de lápiz 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333D9316-CD87-4239-846A-F72DCE9FE053}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId178"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7738680" y="6192360"/>
+              <a:ext cx="145800" cy="302760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>83160</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>166680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>521760</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>106560</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId179">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="450" name="Entrada de lápiz 449">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE20AD3-67B9-458C-ACB9-435DFA2F0F9F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8007960" y="6018840"/>
+            <a:ext cx="2023560" cy="488520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="450" name="Entrada de lápiz 449">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE20AD3-67B9-458C-ACB9-435DFA2F0F9F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId180"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7989960" y="6000840"/>
+              <a:ext cx="2059200" cy="524160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>281460</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>68280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>391620</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152520</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId181">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="130" name="Entrada de lápiz 129">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB3B2347-D7DA-4CE2-93E2-947400CB541D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8206260" y="7932120"/>
+            <a:ext cx="110160" cy="267120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="130" name="Entrada de lápiz 129">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB3B2347-D7DA-4CE2-93E2-947400CB541D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId178"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8188260" y="7914480"/>
+              <a:ext cx="145800" cy="302760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>532740</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>60000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>178860</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>182760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId182">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="131" name="Entrada de lápiz 130">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D10CCEF3-1624-42DB-8F2F-58F5109BB916}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8457540" y="7740960"/>
+            <a:ext cx="2023560" cy="488520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="131" name="Entrada de lápiz 130">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D10CCEF3-1624-42DB-8F2F-58F5109BB916}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId180"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8439540" y="7722960"/>
+              <a:ext cx="2059200" cy="524160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>494880</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>29520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>520800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>44640</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId183">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="473" name="Entrada de lápiz 472">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E87B061A-A708-4844-ADC8-84C7218D3880}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13174560" y="7161840"/>
+            <a:ext cx="2403360" cy="746640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="473" name="Entrada de lápiz 472">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E87B061A-A708-4844-ADC8-84C7218D3880}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId184"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13156560" y="7143840"/>
+              <a:ext cx="2439000" cy="782280"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>470160</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>105480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>633240</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>68040</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId185">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="477" name="Entrada de lápiz 476">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01AF9270-BF33-4DE0-B7E9-57A71AE98CDE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2847600" y="6323400"/>
+            <a:ext cx="163080" cy="145440"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="477" name="Entrada de lápiz 476">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01AF9270-BF33-4DE0-B7E9-57A71AE98CDE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId186"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2829600" y="6305400"/>
+              <a:ext cx="198720" cy="181080"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26559,7 +26819,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">229 242,'-6'2,"0"0,0 0,1 1,-1 0,1 0,0 0,0 1,0 0,0 0,-7 9,1-2,1 0,1 2,0-1,0 1,1 0,1 1,0 0,1 0,1 0,0 1,1 0,-3 22,1 2,3 0,1 0,5 68,-2-93,1 0,0 0,1 1,1-2,0 1,0 0,2-1,13 25,-15-31,0-1,1 1,0-1,0 0,1-1,0 1,0-1,0 0,0-1,1 1,-1-1,1-1,0 1,1-1,-1 0,0-1,16 3,3-1,0-1,1-1,-1-2,1-1,-1-1,0-1,0-1,32-10,-40 9,-2 0,1-2,-1 0,0-1,0 0,-1-2,0 1,-1-2,0 0,0-1,-1 0,-1-1,13-18,-17 21,-1-2,0 1,-1-1,-1 0,0 0,0 0,-1-1,-1 1,0-1,-1 0,0 0,-1 0,-1-26,-1 22,-2 1,0-1,-1 1,-1 0,0 0,-1 0,0 1,-2 0,0 0,-14-20,3 10,-2 1,0 1,-1 0,-2 2,0 1,-1 0,-29-16,-198-96,238 126,-85-36,90 39,0 1,0-1,0 2,-1-1,1 1,0 0,-1 1,1 0,-10 2,4 3,4 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.44">1520 666,'-2'6,"0"-1,1 1,-2 0,1-1,-1 1,1-1,-1 0,-1 0,1 0,-1 0,0-1,-7 7,-10 15,-40 60,-88 169,148-254,0 1,0 0,1 0,-1 0,0 0,1-1,0 1,-1 0,1 0,0 0,0 0,0 4,0-5,0-1,1 1,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,-1-1,1 0,0 1,0-1,0 0,5 1,0 0,-1 0,1-1,0 0,-1 0,12-3,-8 2,31-3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.43">1520 666,'-2'6,"0"-1,1 1,-2 0,1-1,-1 1,1-1,-1 0,-1 0,1 0,-1 0,0-1,-7 7,-10 15,-40 60,-88 169,148-254,0 1,0 0,1 0,-1 0,0 0,1-1,0 1,-1 0,1 0,0 0,0 0,0 4,0-5,0-1,1 1,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,-1-1,1 0,0 1,0-1,0 0,5 1,0 0,-1 0,1-1,0 0,-1 0,12-3,-8 2,31-3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -27836,7 +28096,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">493 157,'0'620,"0"-605,0 0,2 1,0-1,0 0,8 22,-9-34,0 1,1 0,0-1,0 1,0-1,0 0,0 1,1-1,-1 0,1-1,5 6,-6-7,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,1-1,4-1,-3 0,-1 1,1-1,0-1,-1 1,1 0,-1-1,0 0,0 0,0 0,0 0,-1 0,1-1,-1 1,0-1,0 1,0-1,0 0,-1 0,3-6,-1-3,1 0,-2-1,0 1,1-25,-5-209,-1 229,0 1,-1 0,0-1,-2 1,0 1,-12-24,0 5,-42-58,50 81</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1589.56">980 876,'-4'0,"-4"3,-5 2,-4 0,5-1,5-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3120.82">1234 136,'-2'31,"-1"1,-12 48,-2 27,10-13,9 156,-2-241,2-1,-1 0,1 1,1-1,-1 0,1 0,1 0,-1-1,1 1,1-1,-1 0,12 13,-13-17,0 1,1-1,-1 0,1 0,-1-1,1 1,0-1,0 0,0 0,0 0,0-1,1 1,-1-1,1 0,-1 0,0-1,1 1,-1-1,1 0,-1 0,1 0,-1-1,1 0,-1 0,1 0,3-2,-4 2,0-1,-1 0,0 0,1-1,-1 1,0-1,0 1,0-1,-1 0,1 0,-1 0,1-1,-1 1,0 0,0-1,-1 1,3-7,2-8,0-1,3-26,-3 15,-1 7,-2 0,-1-1,0 0,-2 0,-1 0,-1 1,-1-1,-1 1,-1-1,-1 1,-1 1,-1-1,-19-37,14 29,11 26,0-1,0 0,-1 1,1 0,-1-1,0 1,-1 0,1 1,-1-1,-8-7,-9-8,14 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5022.93">1975 136,'-1'1,"1"0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,0-1,1 1,-1-1,0 1,0-1,-2 1,-24 11,19-8,-98 35,54-22,48-15,-1 0,1 1,0-1,0 1,0-1,1 1,-1 1,1-1,-1 0,1 1,0 0,0-1,1 1,-1 0,1 1,0-1,0 0,0 1,1-1,-1 1,1-1,0 1,0 7,-1 10,0 0,2 0,4 37,-4-57,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 0,0 0,1 0,-1 0,0 1,0-1,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 0,0 1,-1-1,1 0,0 0,1 0,6-1,1 0,-1-1,0 0,0 0,14-7,1 1,25-9,-28 9,0 1,0 1,24-3,-38 8,0 0,-1 1,1 0,0 0,0 1,0 0,-1 0,1 0,-1 1,1 0,-1 0,1 1,-1 0,8 5,37 29,-1 3,-2 1,-2 3,42 51,-84-91,1 1,-1 0,0 1,-1-1,1 1,-1-1,0 1,0 0,-1 0,0 0,0 1,0-1,-1 0,0 1,0-1,-1 1,1 0,-1-1,-1 1,0-1,1 1,-2-1,1 0,-1 1,0-1,0 0,-1 0,0 0,0 0,0-1,-1 1,0-1,0 0,0 0,0 0,-1 0,0-1,0 0,-10 6,-9 5,0-1,-1-1,-1-2,-48 16,33-16,0-1,-65 7,78-15,1 0,-1-2,-40-5,53 3,0-1,1-1,-1 0,1-1,0 0,1-1,-1-1,-11-8,5 2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5022.92">1975 136,'-1'1,"1"0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,0-1,1 1,-1-1,0 1,0-1,-2 1,-24 11,19-8,-98 35,54-22,48-15,-1 0,1 1,0-1,0 1,0-1,1 1,-1 1,1-1,-1 0,1 1,0 0,0-1,1 1,-1 0,1 1,0-1,0 0,0 1,1-1,-1 1,1-1,0 1,0 7,-1 10,0 0,2 0,4 37,-4-57,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 0,0 0,1 0,-1 0,0 1,0-1,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 0,0 1,-1-1,1 0,0 0,1 0,6-1,1 0,-1-1,0 0,0 0,14-7,1 1,25-9,-28 9,0 1,0 1,24-3,-38 8,0 0,-1 1,1 0,0 0,0 1,0 0,-1 0,1 0,-1 1,1 0,-1 0,1 1,-1 0,8 5,37 29,-1 3,-2 1,-2 3,42 51,-84-91,1 1,-1 0,0 1,-1-1,1 1,-1-1,0 1,0 0,-1 0,0 0,0 1,0-1,-1 0,0 1,0-1,-1 1,1 0,-1-1,-1 1,0-1,1 1,-2-1,1 0,-1 1,0-1,0 0,-1 0,0 0,0 0,0-1,-1 1,0-1,0 0,0 0,0 0,-1 0,0-1,0 0,-10 6,-9 5,0-1,-1-1,-1-2,-48 16,33-16,0-1,-65 7,78-15,1 0,-1-2,-40-5,53 3,0-1,1-1,-1 0,1-1,0 0,1-1,-1-1,-11-8,5 2</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6619.25">366 1406,'4168'0,"-3704"-7,-5-34,-441 38,-8 3,-1-1,0-1,0 0,-1 0,1-1,0 0,-1 0,1-1,10-6,-17 8,-1 1,1-1,-1 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,0-3,1-37,-1 21,18-136,62-236,-69 343,47-221,11-48,-62 288</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7333.18">5933 30,'-65'159,"23"-48,-123 259,-16 35,179-400,-3 7,0 0,0-1,-10 15,12-23,1 0,-1 1,0-1,0-1,0 1,0 0,-1-1,1 1,-1-1,1 0,-1 0,0-1,-8 3,-65 15,-2-4,-117 7,63-9,-365 46,-320 36,-3-28,-1903-1,2676-67</inkml:trace>
 </inkml:ink>
@@ -28432,7 +28692,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">488 215,'0'3,"0"6,0 7,0 9,0 11,0 10,0 4,3 5,2 3,-1 3,4-5,-1-9,-1-8,2-12,3-9,0-13,2-5,-2-5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="374.98">847 109,'0'3,"3"9,2 13,4 13,3 11,3 7,0 6,0-1,-2-7,-3-9,-4-9,1-10,-1-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="374.97">847 109,'0'3,"3"9,2 13,4 13,3 11,3 7,0 6,0-1,-2-7,-3-9,-4-9,1-10,-1-10</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1000.05">1 236,'38'-47,"-29"34,1 0,14-13,-3 7,1 1,1 1,41-24,-53 34,1 2,-1-1,1 1,1 1,-1 0,0 1,1 0,0 1,0 1,19-1,-22 3,0 1,0 0,-1 1,1 0,-1 0,0 1,1 0,13 10,68 50,-73-50,15 13,-20-16,1 1,1-2,0 0,24 13,-34-21,1 0,-1 0,0-1,0 0,1 0,-1 0,1 0,-1-1,1 0,-1 0,1 0,-1-1,1 0,-1 0,0 0,1-1,-1 0,0 0,7-4,4-4,0-1,0-1,-1-1,0 0,-1-1,15-20,32-29,-43 50,-5 6</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1559.83">128 871,'0'3,"3"2,9 0,13-2,20 0,21-2,27 0,24 0,23-1,18-1,14-6,6-6,-1-2,-17 3,-25 3,-28 3,-28 3,-28 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2087.61">593 1273,'-1'3,"1"6,0 7,0 6,0 9,0 14,4 9,1 4,0-1,2-3,1-8,-2-7,2-10,0-11</inkml:trace>
@@ -28685,7 +28945,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">45 1,'-3'91,"-19"137,10-125,5 1,9 168,0-255,0 1,1 0,1-1,12 32,35 66,-2-2,5 16,-47-109</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="500.27">236 445,'3'3,"5"6,13 7,8 9,15 7,14 13,8 6,11 8,-1 5,-2-4,-7-2,-7-8,-11-7,-13-9,-13-9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1066.84">744 445,'-4'3,"-4"13,-5 17,-4 14,1 14,0 4,2-3,1-4,-2-9,2-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1066.83">744 445,'-4'3,"-4"13,-5 17,-4 14,1 14,0 4,2-3,1-4,-2-9,2-12</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1644.88">1210 741,'-4'0,"-1"3,0 6,1 4,1 7,2 4,0 2,1-1,0 0,0-5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2429.84">1294 64,'2'1,"1"0,0 0,-1 0,1 0,0 1,-1-1,1 1,-1 0,0-1,0 1,0 0,0 1,0-1,0 0,3 5,1 0,16 22,0 0,-2 2,-1 0,16 36,47 139,-72-171,-2 1,-2 0,-1 0,-1 1,-2-1,-2 1,-2-1,-1 1,-1-1,-11 37,11-60,-1 0,-1 0,0-1,-1 0,0 0,-1-1,0 0,-1 0,-16 15,16-18</inkml:trace>
 </inkml:ink>
@@ -28746,7 +29006,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">425 213,'0'-3,"0"0,0 0,0 0,-1 1,1-1,-1 0,1 0,-1 1,0-1,0 0,0 1,0-1,-1 1,1-1,-4-3,3 4,-1 0,0 0,1 0,-1 0,0 1,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 1,-4 0,3 0,0 0,0 0,0 1,0 0,0-1,0 2,0-1,0 0,0 1,1-1,-1 1,1 0,-1 1,1-1,0 0,0 1,0 0,0 0,0 0,0 0,1 0,-4 7,-4 6,0 1,1 0,-10 29,-2 16,3 1,2 0,-10 89,1 199,24 101,4-204,-3-220</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="429.92">1 1186,'3'-4,"9"-4,10-1,0-3,4 1,-2-2,-2-1,-1-3,0 2,-1 3,1 4,-1 4,-3-2,-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="429.91">1 1186,'3'-4,"9"-4,10-1,0-3,4 1,-2-2,-2-1,-1-3,0 2,-1 3,1 4,-1 4,-3-2,-4 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1050.45">784 22,'-92'313,"79"-251,2 1,3 0,1 72,6-83,6 144,-3-173,1 0,2 0,0-1,1 0,1 0,13 28,-15-42,-1 0,1 0,0-1,12 13,0-4</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1519.93">975 403,'3'7,"13"10,10 9,15 11,8 6,7 7,7 2,5 3,1-5,-4-6,-6-4,-12-6,-12-7,-11-10</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2047.36">1483 340,'0'7,"0"9,-4 17,-4 14,-5 9,-4 6,-2 7,1 2,1-6,3-9,4-9,4-13</inkml:trace>
@@ -29309,9 +29569,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-5704.8">636 1186,'-20'-1,"1"2,0 1,0 0,0 1,0 1,1 1,-1 0,-31 16,22-9,17-9,1 2,0 0,1 0,-15 10,21-13,1 0,-1 1,1-1,0 1,0-1,-1 1,2 0,-1 0,0 0,1 0,-1 0,1 1,0-1,0 0,0 1,0-1,1 0,-1 7,1-8,-1 12,1-1,1 1,0-1,2 14,-2-24,0 0,-1 0,1 0,1 0,-1 0,0 0,1 0,-1 0,1-1,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1-1,1 1,0 0,-1 0,1-1,0 0,3 2,17 2,-1-2,1 0,0-1,-1-1,44-5,-17 2,-45 2,-1 0,1 0,-1 0,0-1,1 1,-1-1,0 0,1 0,-1 0,0 0,0 0,0-1,0 0,4-2,-5 2,0-1,-1 1,1-1,-1 1,1-1,-1 0,0 1,0-1,0 0,0 0,-1 0,1 0,-1 0,1 1,-1-1,0-6,-6-160,6 166,-1 0,0 0,1 0,-1 0,0 0,0 1,-1-1,1 0,-1 1,1-1,-1 1,0-1,0 1,0 0,0 0,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,1 0,-1 0,-5-2,-12-2</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-5171.04">1 594,'1'100,"4"-1,5 1,4-2,4 1,33 99,-48-186,1 1,1-1,0-1,1 1,8 14,-12-23,1 0,-1-1,1 1,-1 0,1-1,0 1,0-1,0 0,1 0,-1 0,0-1,1 1,-1-1,1 1,-1-1,1-1,0 1,-1 0,1-1,0 1,0-1,5-1,15-1,-1-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-4657.53">1059 1313,'3'0,"5"-4,5-1,4-3,2 0,6 1,9-2,2 1,2 1,-1 3,-4 1,-3 1,-4-2,-6 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3737.19">1715 975,'-2'0,"1"0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,0 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,0 0,0 2,-9 27,10-29,-4 16,0 0,1 0,1 0,1 1,1 26,0-35,1 0,0-1,1 1,0-1,0 1,1-1,0 0,0 0,1 0,0 0,1-1,9 14,-5-11,1 0,0-1,1 0,0-1,0 0,0-1,1 0,1 0,-1-2,1 1,0-2,0 1,0-2,0 0,1 0,0-2,-1 1,1-2,14 0,-25-1,-1 1,0-1,1 0,-1 0,0 1,0-1,0-1,0 1,0 0,0 0,0-1,0 1,0-1,-1 0,1 1,-1-1,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,-1 0,1-1,0 1,-1 0,1-1,-1 1,0-4,1-10,0 0,-1 0,-4-26,1 11,-6-12,6 30,19 33,-1-2,1-1,0-1,1 0,30 22,-16-14,-29-23,-1 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,-1-1,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,1 3,-2-4,0 1,0 0,0-1,0 1,0-1,0 0,-1 1,1-1,-1 0,1 0,0 1,-1-1,0 0,1-1,-1 1,0 0,1 0,-1-1,-2 1,-30 12,-2-2</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3115.36">276 1779,'1820'24,"-1059"-4,-745-20,-12-1,-1 1,0 0,1 0,-1 0,1 1,-1-1,0 1,1 0,-1 0,0 0,0 0,5 2,-8-2,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,-1 0,1 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 0,0 0,-1 1,1-1,0 0,-1 0,1 0,0 0,0 0,-1 1,-13 7,13-7,-22 10</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2285.54">1313 2245,'-1'-6,"2"1,-1 0,1-1,0 1,0 0,0 0,1 0,0 0,0 0,0 0,0 0,1 0,0 1,4-6,2 0,1 1,0 0,0 0,18-10,-11 6,1 1,1 1,0 1,0 1,33-12,-51 21,0 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 1,1-1,-1 1,0-1,0 1,1 0,-1 0,0 0,0 0,0-1,0 1,0 1,0-1,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 1,-1-1,0 0,1 1,-1-1,0 1,0 1,2 9,-1-1,-1 1,0 0,-2 13,1-7,0-1,1 7,-7 37,6-53,-1 0,0 0,-1 0,0 0,0 0,-1-1,0 1,-7 8,-4 4,-2-1,-1-1,0-1,-1 0,-35 23,-114 61,-138 38,139-67,159-69,-3 2,0 0,0 0,1 1,-16 12,26-18,-1 0,1 1,0-1,-1 0,1 0,0 0,-1 1,1-1,0 0,0 0,-1 1,1-1,0 0,0 1,0-1,-1 0,1 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,0 1,13 3,22-5,-34 0,38-2,392-32,-339 33,1 4,151 22,-203-16</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-933.48">3663 1673,'3'0,"5"0,5 0,7 0,11 3,12 2,11 3,13 1,4 2,-5-1,-7-2,-10-2,-17-3,-18 6,-10 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-576.72">3514 2329,'3'0,"13"0,21 0,22 0,27 0,20 0,17 0,13 0,1 0,-8 0,-22 0,-30-4,-28-1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1104.92">5208 276,'0'-2,"0"1,1 0,-1-1,1 1,-1 0,1 0,-1 0,1-1,0 1,0 0,0 0,-1 0,1 0,0 0,0 0,1 1,-1-1,0 0,0 0,2 0,29-14,-24 12,132-68,-88 43,1 2,85-29,-128 52,0 0,0 1,0 0,1 0,18 1,-25 1,1 1,-1-1,0 1,0 0,1 0,-1 1,0-1,0 1,0 0,-1 0,1 0,0 1,-1-1,0 1,1 0,-1 0,3 3,10 14,0 1,-2 0,23 43,23 75,-39-87,45 84,-63-131,1 0,-1 0,1 0,0 0,0 0,0-1,1 1,-1-1,1 0,0-1,0 1,1-1,10 5,-11-6,1-1,0 0,-1 0,1-1,0 1,0-1,-1-1,1 1,0-1,0 0,-1 0,1 0,-1-1,1 0,5-3,45-21,75-49,-108 61,-5 1,-35 20,-9 8</inkml:trace>
@@ -29319,7 +29577,6 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2198.67">6266 1927,'0'3,"0"9,0 6,0 7,0 10,3 3,2 5,-1 3,4-3,-1-5,-1-5,-1-5,-3-8</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2841.96">6139 2118,'-10'7,"0"1,-1-2,1 1,-1-2,0 1,-1-1,1-1,-1 0,0-1,0 0,0-1,-24 2,29-3,0-1,1 0,-1 0,0-1,0 1,-7-3,13 2,-1 1,0-1,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,1 1,0 0,-1-1,1 1,0-1,0 0,0 1,0-1,0 0,0 1,0-1,1 0,-1 0,1 0,-1 0,1-3,-2-15,1-1,2-29,0 29,0-5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3458.54">5314 2753,'311'-27,"-200"14,215-17,373 13,-687 17,-12 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4213.51">5758 3070,'20'-2,"0"-1,0-1,0 0,-1-1,27-12,6 0,-51 17,11-4,-1 1,0 0,1 1,0 0,15 0,-25 2,0 0,0 1,0-1,0 0,-1 1,1-1,0 1,0-1,0 1,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,1 2,-2-1,0 0,0 0,0 0,0 0,-1 1,1-1,0 0,-1 0,0 0,1 1,-1-1,0 0,0 1,0-1,-1 0,1 0,-1 0,0 4,-3 6,0-1,0 1,-1-1,-1 0,0 0,0-1,-1 0,0 0,-1 0,-10 10,-8 5,-1-1,-36 25,-68 38,-156 76,242-138,38-22,1 1,-1-1,1 2,-10 8,15-13,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,0-1,0 0,-1 0,1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,1 0,-1 0,0 0,0 1,1-1,26 5,307-7,-134-2,-160 3</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -29352,8 +29609,6 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="798.83">2012 531,'3'7,"5"17,5 15,1 15,0 13,-1 10,0-2,2-2,2-7,1-7,-2-10,-7-13,-9-13,-9-11,-8-6,-17-9,-3-3</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1452.29">1060 234,'4'-1,"0"0,0 0,1 0,-1-1,0 1,0-1,0 0,0 0,0-1,-1 1,5-4,7-5,73-46,-50 30,1 2,1 2,74-31,-108 51,0 1,0 0,1 0,-1 1,1 0,-1 0,1 1,0 0,-1 0,1 0,-1 1,1 0,0 0,-1 1,0-1,1 2,-1-1,0 1,0-1,0 2,-1-1,1 1,-1 0,0 0,0 0,7 7,29 32,37 49,16 16,-67-79,1-1,1-1,2-2,1-1,47 27,-69-45,1-1,0 0,0 0,0-2,1 1,0-1,-1-1,1 0,0-1,0 0,0-1,0 0,0 0,0-2,0 1,-1-2,1 0,-1 0,1-1,-1 0,0-1,13-7,3-5,-1-2,-1 0,26-25,63-73,-62 60,-46 52</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1971.02">1123 1801,'7'0,"2"-4,11-5,13-4,18-3,19-7,30-3,23-7,23-3,11 3,9 5,-6 9,-9 7,-23 5,-26 5,-27 2,-26 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2612.71">2203 1716,'-19'9,"1"0,0 2,1 0,0 1,0 1,2 1,-19 20,27-26,0 0,1 1,0 0,1 0,0 0,1 1,0 0,0 0,1 0,0 0,1 0,0 1,0-1,1 1,1-1,0 12,0-19,1 0,-1 1,1-1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,0-1,1 0,-1 1,1-1,-1 0,1 0,0-1,0 1,-1 0,1-1,1 0,-1 0,0 0,0 0,6 1,10 1,0-1,1 0,38-3,-34 1,-4 0,-1-1,1-1,0-1,-1-1,0 0,1-1,-2-2,20-8,-32 13,1-2,-1 1,0-1,-1 0,1 0,0 0,-1-1,0 0,0 0,-1 0,1-1,-1 0,-1 0,1 0,-1 0,0 0,0-1,0 1,-1-1,0 0,-1 0,1 1,-1-1,-1 0,1-13,-2 15,0 0,0 1,0-1,0 0,-1 1,0-1,0 1,0 0,0 0,-1 0,0 0,1 0,-1 0,-1 1,1 0,0-1,-1 1,0 0,0 1,-7-5,-9-4,0 1,-1 0,-22-6,33 13,-36-14,0 3,-2 2,-82-11,105 21,0 0,0 2,-1 1,1 1,0 1,0 1,1 1,-47 16,32-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3442.16">1906 2118,'-4'0,"1"0,0 1,0 0,-1 0,1 0,0 0,0 0,0 0,0 1,1-1,-1 1,0 0,0 0,1 0,0 0,-1 1,1-1,0 1,0-1,0 1,0 0,1 0,-3 4,0 1,1 0,0 0,0 0,1 1,0-1,0 1,0 13,2-17,0-1,0 0,0 0,1 0,0 0,0 0,0 0,0 0,1 0,0 0,0 0,0-1,0 1,3 3,0-1,0 0,0-1,1 0,0 0,0 0,0-1,9 5,5 0,-1 0,1-2,1 0,33 6,24-1,1-4,-1-4,145-10,-216 6,0 0,-1-1,1 0,0 0,0-1,-1 0,1 0,-1-1,8-4,-11 6,-1-1,1 0,-1 0,0 0,0-1,0 1,0 0,0-1,0 1,-1-1,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0-5,0-3,0 0,0-1,-2 1,-3-16,4 24,0-1,0 1,0 0,-1-1,0 1,1 0,-1 0,0 0,0 0,-1 1,1-1,-1 0,1 1,-1 0,0 0,0 0,0 0,-4-2,-11-4,-1 2,1 0,-1 1,-38-6,-81 2,122 9,0 0,0 1,0 1,0 1,0 0,0 1,1 1,-19 7,24-7,1-1,0 2,1-1,-1 1,1 0,0 1,1 0,-1 0,1 1,1 0,-1 0,2 0,-10 18,-11 33,17-35</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -29502,7 +29757,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">424 21,'24'-2,"44"-6,-45 4,0 1,30 0,-50 3,0 0,0 0,0 1,0 0,0-1,0 1,0 0,0 1,0-1,-1 0,1 1,0 0,-1-1,1 1,-1 0,4 4,-2-2,0 1,0 1,-1-1,0 0,0 1,0 0,3 10,0 6,0 0,-2 1,2 31,-5-46,0 0,-1-1,0 1,0 0,-1 0,0 0,0-1,-4 10,4-13,-1 0,0-1,-1 1,1 0,-1 0,1-1,-1 0,0 1,0-1,-1 0,1 0,-1-1,1 1,-1-1,-6 3,0 0,-19 10,29-15,-1 0,1 0,0 1,-1-1,1 0,0 1,-1-1,1 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 0,0 1,0-1,1 1,-1-1,0 0,0 0,1 1,-1-1,0 0,1 1,-1-1,0 0,1 0,-1 0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,20 10,33 9,-38-15,-1 1,-1 1,1 0,-1 1,23 15,-31-19,-1 1,0 1,0-1,0 1,0 0,-1 0,0 0,6 11,-9-14,0 0,-1-1,1 1,-1 0,1 0,-1 0,0 0,0 0,0 0,0 0,0-1,0 1,0 0,-1 0,1 0,-1 0,1 0,-1-1,0 1,1 0,-1-1,0 1,0 0,-1-1,1 1,0-1,0 1,-1-1,1 0,-1 0,1 0,-1 1,1-1,-1-1,-2 2,-13 9,0-1,0-1,-1 0,0-2,0 0,-1-1,0-1,0 0,0-2,-1 0,-25 0,41-3,1 0,0 0,0 0,0 0,-1 0,1 0,0 1,0-1,0 1,0 0,0 0,0 0,0 1,-5 2,0 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="514.55">1 1016,'41'-3,"1"-1,-1-2,47-13,33-6,288-8,5 34,-246 1,-26 0,-117-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="514.54">1 1016,'41'-3,"1"-1,-1-2,47-13,33-6,288-8,5 34,-246 1,-26 0,-117-2</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1229.53">551 1080,'-1'2,"0"0,0 1,0-1,0 0,0 1,0-1,-1 0,1 0,-1 0,0 0,1-1,-1 1,0 0,-4 2,-10 13,12-8,-1-1,2 1,-1 1,1-1,1 0,0 1,0 0,0-1,1 13,0-2,1 0,1 0,6 32,-5-45,-1-1,1 1,1 0,0-1,0 0,0 1,0-1,1 0,0-1,0 1,1-1,0 1,0-1,0-1,0 1,1-1,0 0,0 0,0-1,0 1,10 2,-2-1,0 0,0-2,0 0,1 0,-1-1,1-1,0-1,-1 0,20-2,-29 1,-1 0,0 0,0-1,0 1,0-1,0 0,0 0,-1 0,1 0,0-1,-1 0,0 1,0-1,0 0,0-1,0 1,0 0,-1-1,0 0,0 1,0-1,0 0,0 0,-1 0,2-5,0-3,0-1,0 0,-2 1,1-1,-1 0,-1 0,-2-17,0 22,0 0,0-1,-1 2,0-1,-1 0,1 1,-1-1,-1 1,0 0,0 1,0-1,-1 1,1 0,-1 0,-1 1,1-1,-1 2,0-1,-8-4,-1 0,-1 1,0 0,0 1,0 1,-1 1,0 0,-31-4,46 9,-1-1,-1 0,1 0,0 1,0 0,-1 0,1 0,0 0,0 1,-1-1,1 1,0 0,0 1,0-1,0 1,0-1,0 1,-3 3,-2 5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1965.56">509 1397,'-8'0,"1"1,0 1,0-1,0 1,0 1,0-1,1 1,-1 0,1 1,-1-1,1 1,0 0,1 1,-1 0,1 0,0 0,0 0,0 1,1 0,0 0,0 0,0 0,1 1,0-1,0 1,1 0,0 0,0 0,1 0,-2 10,2 39,6 58,-5-109,1-1,0 1,-1-1,2 1,-1-1,1 0,-1 1,1-1,0 0,1 0,-1 0,1-1,-1 1,1-1,7 7,-4-5,0-1,1 1,0-1,0 0,0-1,0 0,1 0,11 3,10 0,1-2,-1 0,54-2,-75-2,8 1,1-2,-1 0,0-1,0 0,0-1,0-1,19-8,-26 8,-1 0,0 0,0-1,0 0,-1-1,1 0,-2 0,1-1,0 1,-1-1,-1-1,1 1,-1-1,5-9,-4 4,0 0,-1 1,6-25,-9 32,-1 0,0-1,0 1,-1-1,0 1,0-1,0 1,0-1,-1 1,0-1,0 1,-2-7,2 11,-1-1,1 0,0 0,0 1,-1-1,1 0,-1 1,1 0,-1-1,0 1,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,-3-1,-48 0,44 1,-10 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2822.68">1207 1164,'-6'6,"0"2,1-1,0 0,1 1,0 0,0 0,1 0,0 0,0 1,-2 13,-1 10,-3 45,7-57,1-8,-1-1,2 0,-1 0,1 0,1 1,0-1,6 21,-6-29,1-1,0 0,-1 0,1 0,1 0,-1 0,0-1,0 1,0-1,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1-1,0 1,0-1,-1 0,1 0,0 0,4 0,6 0,0-1,0 0,22-6,-29 6,0-1,0 0,0 0,0-1,0 1,0-1,-1 0,0-1,1 0,-1 1,0-2,-1 1,1 0,-1-1,0 0,6-10,-5 7,-1-1,-1-1,1 1,-2 0,1-1,-1 0,-1 1,0-1,0 0,-1-13,-5-143,4 163,1-1,0 1,-1 0,0 0,0-1,0 1,0 0,0 0,-1 0,1 0,-1 0,0 1,0-1,0 0,0 1,0-1,0 1,-5-4,3 4,-1 0,1-1,0 1,-1 1,0-1,1 1,-1-1,0 2,0-1,0 0,-7 1,0 0,1 1,-1 0,1 1,-1 0,1 1,0 0,0 1,0 0,1 1,-12 6,15-5,-1 0,1 0,-1 0,2 1,-8 8,-6 11</inkml:trace>
@@ -29668,141 +29923,6 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:25:41.411"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 179,'-3'-1,"0"1,0 0,0 1,1-1,-1 0,0 1,1-1,-1 1,0 0,1 0,-1 0,1 0,-1 0,1 1,0-1,-3 3,3-1,0-1,0 1,1 0,-1-1,1 1,-1 0,1 0,0 0,0 0,0 0,1 1,-1-1,1 0,0 3,-2 12,1-1,1 1,1-1,0 1,2-1,0 0,0 0,13 32,-13-41,0-2,0 1,1 0,0-1,0 1,1-1,-1 0,1-1,1 1,-1-1,1 0,0 0,0-1,0 0,1 0,0 0,-1-1,1 0,1 0,-1-1,0 0,14 2,-16-3,0 0,-1-1,1 1,0-1,0 0,0-1,-1 1,1-1,0 0,-1 0,8-3,-8 2,-1 0,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,-1 0,0-1,0 1,0 0,0-1,2-5,7-20,-1 0,-2-1,-1 0,-1-1,-2 1,-1-1,-1 0,-3-40,2 196,5 141,-5-251,5 62,19 101,-16-145</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="719.18">787 793,'-1'3,"-2"2,-6 3,-4 0,-3 0,0-7,7-2,12-5,13-5,7-1,0 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1600.1">914 264,'0'-2,"0"0,1 1,-1-1,1 0,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0 0,1 0,-1 0,3-2,32-18,-27 17,27-16,1 3,0 0,1 3,1 1,0 2,1 2,63-7,-101 16,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,-1-1,1 1,-1 0,0-1,2 4,-1 1,0 0,0 1,-1-1,0 0,-1 1,1-1,-1 1,-1 7,1 3,-1 1,-1-1,-1 1,0-1,-1 0,-1 0,-1 0,0-1,-1 0,-1 0,0-1,-2 1,1-2,-2 0,0 0,0-1,-19 16,25-24,-14 14,19-18,0-1,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 0,1 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,105 24,-29-8,0 4,114 45,-180-61,-1 1,0 0,-1 1,1 0,-1 0,11 11,-18-15,-1-1,0 0,1 1,-1-1,0 1,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0 0,-1 0,1 0,-1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,0 0,0 0,0 0,1-1,-2 1,1-1,0 1,0-1,0 1,-1-1,1 0,-1 1,1-1,-1 0,-2 1,-5 4,1-1,-1 0,0-1,0 0,-1 0,1-1,-1 0,1-1,-1 0,-10 1,-20 0,-46-1,58-3,-15 1,7-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2459.33">1782 200,'12'-2,"0"1,0-2,0 0,0 0,0-1,-1 0,22-12,9-3,274-91,-313 109,8-3,0 1,0 0,0 1,1 0,18 0,-27 2,-1 0,0 0,1 1,-1-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 1,0-1,1 0,-1 3,1 9,-1 0,0 0,-1-1,0 1,-1 0,-1-1,0 1,-1-1,-1 0,0 0,0 0,-1-1,-1 1,-14 19,4-10,-1 0,0-1,-2-1,0-1,-1 0,-31 19,-9 1,61-39,0 0,0 0,1 0,-1 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 0,0 0,0 1,0-1,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,0 0,-1 1,38 2,-22-2,43 7,-1 3,-1 3,0 2,0 2,-2 3,89 47,-139-66,0 0,0 1,0-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,-1 1,1-1,-1 1,1 0,-1 0,2 5,-3-6,-1-1,0 0,1 0,-1 1,0-1,-1 0,1 0,0 1,0-1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,-1 1,0 0,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,-3 2,-14 6,1-1,-1-1,-1-1,1-1,-1 0,-26 2,-121 3,162-10,-22 0,26 0,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1 0,0 0,-1 0,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,1 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,0-1,0 1,0 0,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,1 0,5-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3179.11">3242 31,'-44'-17,"41"16,-3-2,-1 1,0 0,0 0,0 1,-1 0,-13-1,18 3,0-1,0 1,0 0,1 0,-1 0,0 1,0-1,1 1,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,0 1,0-1,0 0,-2 6,-1 1,0 0,1 1,0 0,0 0,1 0,0 0,-2 19,4-22,1 0,-1 0,1 0,0 0,0 0,1 0,0 0,0 0,1 0,0 0,0 0,5 9,-4-12,0-1,0 1,0-1,1 1,0-1,-1 0,1 0,0-1,0 1,0-1,1 0,-1 0,1 0,-1-1,1 0,8 2,9 0,0 0,28-1,-37-2,28 2,-12 0,-1-1,1-1,0-2,40-7,-65 7,0 0,0 0,0 0,0 0,0-1,-1 1,1-1,-1 0,1 0,-1 0,0-1,0 1,0-1,-1 0,1 1,3-9,-4 8,0 0,-1 0,1 0,-1 0,0 0,0 0,0 0,0-1,-1 1,0 0,0 0,0-1,0 1,-1 0,0 0,1 0,-1-1,-2-3,0 4,0 1,0 0,0 0,0 0,-1 1,1-1,-1 1,1 0,-1 0,0 0,0 0,0 1,0 0,0-1,-6 0,-4-2,-28-9,-1 2,0 1,-1 3,-67-3,79 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3932.6">3327 370,'-4'-1,"0"0,0 0,0 0,1 0,-1 0,0-1,1 0,-5-2,-9-5,8 6,-2-2,1 1,-2 0,1 0,0 1,-1 1,-13-2,22 4,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1 0,1 0,0 0,0 1,-1 0,1 0,0-1,0 2,1-1,-1 0,0 0,1 1,-1 0,1-1,0 1,0 0,0 0,-3 6,1 1,0-1,0 1,1-1,0 1,0 0,1 0,-1 16,2 72,2-88,-2-6,1 0,0-1,1 1,-1 0,1 0,0-1,-1 1,2 0,-1-1,0 1,1-1,-1 0,1 1,0-1,0 0,0 0,1 0,-1 0,1 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1-1,1 0,-1 1,1-1,-1 0,5 0,30 4,0-2,0-1,50-4,-31 1,-47 0,15 2,-1-2,1-1,-1-1,43-10,-62 11,0 1,0-1,0 0,0-1,0 1,0-1,-1 0,0 0,1 0,-1 0,0-1,-1 0,1 0,-1 0,1 0,-1-1,0 1,-1-1,1 0,-1 1,0-1,0 0,-1 0,1-1,-1 1,0 0,0-11,0 9,-1 0,0 0,0 0,-1 0,0 0,0 0,0 0,-4-9,3 12,-1 0,1 0,0 0,-1 0,0 0,0 1,0 0,-1-1,1 1,-1 1,1-1,-1 0,0 1,-6-3,-29-14,-1 2,-1 1,-51-11,-134-17,190 38,-1 2,0 2,0 1,0 2,0 1,1 2,-1 2,1 1,-48 17,15 5</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink308.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:25:46.626"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 825,'-1'3,"1"6,0 3,4 5,8-1,9 0,2 1,7 5,5 2,5 1,3 3,0 1,1-2,-4-1,-5-5,-8-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="438.33">340 656,'0'3,"-4"2,-1 3,-7 8,-5 4,0 10,0 7,-4 8,-3 3,-1-2,4-3,2-7,5-8,4-3,7-8,8-5,7-6,1-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1037.41">594 677,'0'3,"0"9,0 13,0 9,3 10,2 9,3 1,0 3,3-1,-1-6,2-9,-2-6,-2-7,1-8,3-7,2-6,0-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1611.9">953 656,'-1'0,"0"1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 2,-10 24,10-25,-17 55,3 1,3 0,-9 118,20-174,0 1,0 0,0 0,0 0,1-1,-1 1,1 0,-1 0,1-1,0 1,0 0,0-1,1 1,-1-1,0 1,1-1,0 0,0 0,-1 0,4 3,-1-3,0 0,0 1,1-1,-1-1,1 1,0-1,-1 1,1-2,0 1,-1 0,7-1,31 3,80-5,-107 1,0-1,0 0,-1-2,1 1,-1-2,0 0,0 0,24-15,-33 17,-1-1,0 1,0-1,0 0,0 0,-1-1,0 1,0-1,0 1,0-1,-1 0,1 0,-1 0,-1-1,1 1,-1 0,1-7,0 0,-1 0,-1 1,0-1,-1 1,0-1,0 0,-5-14,4 20,-1 0,1 0,-1 1,-1-1,1 1,-1-1,1 1,-2 1,1-1,0 0,-1 1,-5-4,-3-2,-1 0,0 1,-21-10,2 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2389.84">1165 380,'36'-12,"-18"5,-82-5,-191-40,246 49,20 2,3 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3268.13">1229 105,'0'-2,"0"0,1 0,-1 1,1-1,-1 0,1 1,0-1,0 0,0 1,0-1,0 1,0-1,0 1,1 0,-1-1,0 1,3-1,30-21,-25 18,3-2,0 0,0 1,1 1,0 0,0 1,0 0,1 1,-1 0,1 1,0 1,0 0,26 2,-38 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,2 2,-1 0,0 1,-1-1,1 1,-1-1,1 1,-1-1,-1 1,1 6,0-1,-1 1,-1-1,0 0,0 1,-1-1,0 0,-6 14,4-15,-1 0,0 0,-1 0,0-1,0 0,-1 0,0 0,0-1,-1 0,0-1,0 0,0 0,-1 0,0-1,0-1,-1 1,1-2,-12 4,34-9,0 1,0 0,0 1,0 0,22 4,85 18,-90-15,-1 2,0 1,-1 1,0 1,-1 2,42 27,-66-39,0 1,0-1,0 1,0 0,-1 0,1 0,-1 0,0 0,1 0,-1 1,-1-1,1 1,2 5,-4-7,0 0,0-1,0 1,0 0,0 0,-1-1,1 1,0 0,-1-1,1 1,-1 0,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,-2 0,-27 10,-1 0,0-2,0-2,-1-1,-65 4,72-9</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink309.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:25:51.322"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">261 22,'-4'0,"-4"0,-5 0,-4 0,-2-4,-2-1,-1 1,0 0,0 2,0 0,0 1,1 4,3 6,1 4,4 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink31.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-05-30T14:57:41.881"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#AB008B"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1096,'3073'0,"-2412"30,-636-28,-6-1,0 0,-1 2,1 0,0 1,-1 0,19 8,-36-12,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 0,1 1,-1-1,1 0,-1 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,-1 1,1 0,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,-1 0,1 1,-1 0,-10 7,-1 0,0-1,-1-1,1 0,-1-1,0 0,-22 5,-5 4,-83 29</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1237.36">469 1553,'16'0,"-1"-2,1 0,0 0,-1 0,1-2,22-9,86-43,-77 33,174-81,-217 101,1 1,-1 1,0-1,1 0,0 1,0 0,0 0,-1 1,1-1,1 1,-2 0,7 0,-8 1,-1 0,2 0,-2 0,0 1,0-1,0 1,1-1,-1 1,-1-1,1 1,0-1,0 1,-1 0,1 0,-1 0,2 1,-2-1,0 0,0 1,0-1,0 0,-1 1,2 3,4 18,-2-1,0 1,-1 0,-1 27,-11 105,3-68,5-67,-5 103,-24 127,20-204</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2546.39">1598 2037</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4403.39">2314 1375,'-14'16,"1"0,1 0,1 2,1-1,-1 0,3 2,0 0,-7 22,-1 0,-6 16,2 1,2 0,3 0,4 2,2-1,2 2,5 96,2-155,0 0,1 1,-1-1,1 1,0 0,-1-1,2 1,-1-1,0 1,1-2,-1 1,0 0,1 1,0-1,-1 0,1 0,0 0,0-1,3 4,1-3,-2 0,1 0,-1-1,1 1,1 0,-2-1,1 0,0 0,10 0,7 0,-2-2,2-1,-1 0,23-5,-26 3,1-1,0-1,28-11,-42 15,1-1,-1 1,1-1,-1-1,0 1,0 0,-1 0,0-1,2-1,-2 1,-1-1,1 2,-1-2,1 0,3-7,-6 8,-1 0,1 0,-1 0,0 0,0 0,0 1,-1-1,0 0,1 0,-1 0,-1 0,0 0,0 1,1-1,-1 1,0-1,0 1,-1-1,1 1,-1 1,0-1,1 0,-2 0,-3-2,-9-8,-1-1,-1 3,-22-13,31 19,0 0,1 1,-2 1,1-1,0 3,-1-2,1 1,-1 0,-9 0,-3 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5752.48">2864 1476,'-19'22,"1"1,1 1,2 0,0 0,-18 44,-8 11,23-49,9-16,1-1,0 1,1 0,0 1,2 0,-8 29,13-42,0 0,0 1,1-1,-1 0,1 0,-1 0,1 0,0-1,1 1,-1 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,-1 1,1-1,0 1,0-1,0-1,0 1,1 0,-1 0,0 0,0-1,0 1,0-1,4 1,11 3,-1-1,1-1,21 1,-27-2,75 1,-62-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6385.49">3057 1426,'-5'0,"-6"9,-1 11,1 11,-2 13,-3 13,-5 4,-7 10,-7 2,0 0,2 2,8-4,8-10,5-6,11-13,5-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7480.49">3277 1604,'-10'22,"2"0,-1 0,-4 34,-5 9,9-38,-2 2,2 1,2-1,1 1,0 0,2 0,1 39,4-66,0 1,0 0,0-1,0 1,0 0,1-1,-1 0,1 0,1 0,-1 1,0-1,1 0,-1 0,1 0,0-2,0 2,0-1,1 1,-1-1,0 0,0 0,1 0,-1-1,1 1,1-1,-2 0,7 1,-6-1,-1-1,1 0,1 1,-2-1,1 0,0 0,-1 0,1 0,1-1,-2 1,1 0,0-1,-1-1,1 1,-1 0,1-1,0 0,-1 0,0 0,0 0,0 0,0 0,0-1,-1 0,2 2,-2-2,0 0,3-5,0-2,-1 1,-1-2,1 2,-1-2,-1 2,0-2,0-16,-5-80,0 52,4 48,-1 0,0-1,-1 2,0-1,0-1,0 2,-2-1,1 0,0 0,-1 1,0-1,0 0,-1 1,0 1,-1-1,-8-10,-10-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8891.49">3801 1604,'0'0,"0"0,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1-1,-1 1,-14 5,-14 18,16-11,1-1,0 2,1-1,0 2,2 0,-1 1,2-1,-13 28,22-41,-1 1,1 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 0,0 0,1 1,-1-1,0 0,1-1,-1 1,2 1,9 3,0-1,-1 1,19 4,11 5,-26-5,-1 0,0 0,-2 1,1 0,-1 1,0 0,-1 2,0-1,-2 1,0 0,9 17,-12-19,-1-1,1 2,-2-1,0 1,-1-1,0 1,-1 0,0 0,-1 1,-1-2,0 2,0-1,-1 0,-1-1,-3 13,3-20,1-1,-1 0,1 0,-1 0,0-1,-1 1,1 0,-1-1,0 1,1-1,-1 0,0 1,0-1,0 0,0-1,-1 0,1 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,0-1,-6 1,-12 0,1-1,-1 0,-25-5,30 4,7 0,-1 0,1-1,0 1,0-2,1 0,-2 0,2-1,0 0,-12-7,-2-6</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9612.49">4957 968,'-15'5,"-8"5,-19 23,-46 40,-30 12,-19 10,4-4,12-13,21-15,27-22,27-19</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10249.49">4186 1045,'4'0,"7"0,10 0,13 17,2 15,2 14,3 13,0 5,-8-5,0 2,-1-6,-5-8,-3-11,-6-5,-1-6,6-16,-2-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10757.59">5122 968,'0'22,"0"20,0 20,0 8,0 1,-5 11,-1-6,0-6,-4 2,1-8,0-4,8-14,13-18,5-15</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11960.59">5645 1147,'0'0,"0"-1,0 1,0-1,0 1,0-1,0 1,-2-1,2 1,0-1,0 1,0-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1-1,0 1,-1 0,1-1,0 1,-1 0,1-1,-1 1,1 0,0-1,-1 1,1 0,-1 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 1,-1-1,1 0,0 1,-1-1,1 1,0-1,-1 1,-30 23,2 9,2 1,2 1,1 1,-32 67,48-85,1 0,0 1,2-1,0 1,1 0,1 0,1 0,1 1,1 0,1-1,0 0,8 35,-8-50,1 0,-1 0,1 0,0 0,0 0,2 0,-2 0,1-1,0 1,0-1,0 0,0 1,0-1,1 0,0-1,0 0,0 0,0 1,0-1,0 0,2-1,-2 1,0-1,1 0,8 1,10 1,-1-2,0 0,1-2,29-3,-20 1,-19 2,-1 0,1-1,-2 0,2-1,-2-1,2 1,-2-1,1-1,-2 0,21-12,-25 12,2-1,-2 1,-1 0,1-1,0 0,-1-1,0 1,-1-1,0 0,1 0,-2 1,0-2,0 0,-1 1,0-1,2-13,-1 2,-2-1,0 1,-1 0,-2 0,1 0,-2 0,-1 0,-1 1,0-1,-13-26,14 36,0 0,-2 0,0 1,1-1,-1 1,-2 1,2-1,-1 1,-1 1,0-1,0 0,-1 1,0 1,0 0,0 0,-1 0,0 1,0 0,0 2,0-1,-22-4,28 7,-1 0,1 0,-1 0,1 0,-2 0,2 1,-1 0,1 0,-1 0,0 0,1 1,-6 3,-14 8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13395.59">6196 1197,'-3'30,"-1"1,-1 0,-3-1,-12 34,8-23,-9 25,13-44,0 1,1 0,1 1,2-1,1 1,1 0,1 32,1-53,0-1,0 1,1-1,-1-1,1 2,0-1,-1 0,1 0,0 1,0-1,0 0,1 0,-1 0,1 0,-1-1,1 0,-1 1,1 0,0-1,1 1,-1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,1-1,0 1,0-1,-1 0,0 0,1 0,-1 0,1-1,2 0,3 0,-1 0,0-1,1 0,-2 0,1-1,0 0,0 0,-1 1,0-2,0 0,1 0,4-6,-3 2,0-1,-1 0,-1-1,0 0,1 0,-2-1,-1 2,0-3,0 1,4-21,0-11,1-62,-7 79,-1 1,-2 0,-4-34,4 53,0 1,0-1,0 0,-1 1,0 0,0 0,0-1,-1 1,-1 0,1 1,0-1,-1 0,1 1,-1-1,0 1,-1 1,0-1,1 0,-1 1,0 0,-7-4,-10 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14169.59">6939 1147,'9'0,"8"0,6 0,3 0,12-4,8-2,11 0,19 1,20 3,44 0,9 1,-16 0,-26 1,-33 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15107.59">6718 1375,'1099'0,"-998"5,1 4,-1 3,142 36,-183-34</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31543.89">12609 994,'-5'13,"-20"17,-14 12,-16 17,-22 24,-7 6,7-3,11-12,8-14,13-13,9-10,12-12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32777.17">12032 739,'-17'1,"1"0,-1 0,1 1,0 1,0 1,0-1,0 2,1 1,0 0,0 1,-20 12,29-15,0-1,0 1,1 0,0 1,0 0,0 0,1-1,0 2,0 0,0-1,1 0,-1 2,1-1,0 0,1 0,0 0,1 1,-1 0,1-2,0 2,1 0,0 0,0-1,0 1,1-1,0 1,0-1,4 12,-3-14,0 1,1 0,0 0,0 0,0-1,0 0,1 1,-1-1,1 0,1 0,-1-1,0 0,0 1,1-1,10 5,-4-3,1 0,0-1,0 0,0 0,1-1,13 2,-23-5,0 0,0-1,0 1,0 0,0-1,0 0,1 0,-1 0,-1 0,1 0,0 0,-1-1,1 1,0-1,-1 0,1 0,0 0,-1 0,0 0,0 1,0-2,-1 1,1 0,0-1,-1 0,0 1,2-6,5-5,-2-2,-1 0,7-25,-5-2,-2 1,-2 0,-4-61,0 75</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34704.17">12638 1476,'-6'1,"2"0,0 0,0 0,-1 1,1-1,-1 1,1 0,0 0,1 0,-1 0,0 1,0-1,1 1,0 0,0 0,0 0,0 0,0 1,-2 4,-10 12,2 1,-11 26,14-30,-2 7,-53 107,58-114,0 1,1 1,1-1,2 0,-3 28,6-42,0 0,1-1,-1 1,1 0,0-2,0 2,0-1,0 1,1-1,0 0,-1 1,1-1,0-1,1 1,0 0,-1 0,1-1,-1 1,1-1,0 1,0-1,0 0,1-1,-1 0,1 1,-1 0,1-1,6 2,2 0,-1 0,1 0,0-2,0 1,0-1,0-1,0 0,14-2,-22 1,1-1,0 1,-1-1,-1 0,1 0,0 0,0-1,0 1,0-1,-1 1,0-1,0 0,0-1,0 1,-1-1,2 1,-2-1,0 1,0-1,2-4,4-11,1 1,7-35,-8 14,-3 1,-1-1,-3 1,-4-65,-1 5,5 92,0 1,-1-2,-1 1,1-1,-1 2,0-2,0 1,-1 0,0 1,0-1,-1 0,1 0,-1 0,0 1,-1 0,1-1,-1 1,-9-7,-2 2</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink310.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:25:55.730"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -29822,98 +29942,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink311.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:26:11.673"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 179,'-3'-1,"0"1,0 0,0 1,1-1,-1 0,0 1,1-1,-1 1,0 0,1 0,-1 0,1 0,-1 0,1 1,0-1,-3 3,3-1,0-1,0 1,1 0,-1-1,1 1,-1 0,1 0,0 0,0 0,0 0,1 1,-1-1,1 0,0 3,-2 12,1-1,1 1,1-1,0 1,2-1,0 0,0 0,13 32,-13-41,0-2,0 1,1 0,0-1,0 1,1-1,-1 0,1-1,1 1,-1-1,1 0,0 0,0-1,0 0,1 0,0 0,-1-1,1 0,1 0,-1-1,0 0,14 2,-16-3,0 0,-1-1,1 1,0-1,0 0,0-1,-1 1,1-1,0 0,-1 0,8-3,-8 2,-1 0,0-1,0 1,0-1,0 1,0-1,-1 0,1 0,-1 0,0-1,0 1,0 0,0-1,2-5,7-20,-1 0,-2-1,-1 0,-1-1,-2 1,-1-1,-1 0,-3-40,2 196,5 141,-5-251,5 62,19 101,-16-145</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">787 793,'-1'3,"-2"2,-6 3,-4 0,-3 0,0-7,7-2,12-5,13-5,7-1,0 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">914 264,'0'-2,"0"0,1 1,-1-1,1 0,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0 0,0 0,1 0,-1 0,3-2,32-18,-27 17,27-16,1 3,0 0,1 3,1 1,0 2,1 2,63-7,-101 16,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 1,0-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,-1-1,1 1,-1 0,0-1,2 4,-1 1,0 0,0 1,-1-1,0 0,-1 1,1-1,-1 1,-1 7,1 3,-1 1,-1-1,-1 1,0-1,-1 0,-1 0,-1 0,0-1,-1 0,-1 0,0-1,-2 1,1-2,-2 0,0 0,0-1,-19 16,25-24,-14 14,19-18,0-1,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 0,1 0,-1 1,1-1,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,105 24,-29-8,0 4,114 45,-180-61,-1 1,0 0,-1 1,1 0,-1 0,11 11,-18-15,-1-1,0 0,1 1,-1-1,0 1,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,0 0,-1 0,1 0,-1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,0 0,0 0,0 0,1-1,-2 1,1-1,0 1,0-1,0 1,-1-1,1 0,-1 1,1-1,-1 0,-2 1,-5 4,1-1,-1 0,0-1,0 0,-1 0,1-1,-1 0,1-1,-1 0,-10 1,-20 0,-46-1,58-3,-15 1,7-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1782 200,'12'-2,"0"1,0-2,0 0,0 0,0-1,-1 0,22-12,9-3,274-91,-313 109,8-3,0 1,0 0,0 1,1 0,18 0,-27 2,-1 0,0 0,1 1,-1-1,0 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,0-1,-1 1,1-1,0 1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 1,-1-1,1 0,-1 1,0-1,1 0,-1 3,1 9,-1 0,0 0,-1-1,0 1,-1 0,-1-1,0 1,-1-1,-1 0,0 0,0 0,-1-1,-1 1,-14 19,4-10,-1 0,0-1,-2-1,0-1,-1 0,-31 19,-9 1,61-39,0 0,0 0,1 0,-1 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 0,0 0,0 1,0-1,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,0 0,-1 1,38 2,-22-2,43 7,-1 3,-1 3,0 2,0 2,-2 3,89 47,-139-66,0 0,0 1,0-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,-1 1,1-1,-1 1,1 0,-1 0,2 5,-3-6,-1-1,0 0,1 0,-1 1,0-1,-1 0,1 0,0 1,0-1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0-1,-1 1,0 0,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,-3 2,-14 6,1-1,-1-1,-1-1,1-1,-1 0,-26 2,-121 3,162-10,-22 0,26 0,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,-1 1,1 0,0 0,-1 0,1 0,-1-1,1 1,0 0,-1 0,1-1,0 1,-1 0,1 0,0-1,-1 1,1 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,0-1,0 1,0 0,-1-1,1 1,0-1,0 1,0-1,0 1,0-1,1 0,5-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">3242 31,'-44'-17,"41"16,-3-2,-1 1,0 0,0 0,0 1,-1 0,-13-1,18 3,0-1,0 1,0 0,1 0,-1 0,0 1,0-1,1 1,-1-1,1 1,0 0,-1 0,1 0,0 0,0 0,0 1,0-1,0 0,-2 6,-1 1,0 0,1 1,0 0,0 0,1 0,0 0,-2 19,4-22,1 0,-1 0,1 0,0 0,0 0,1 0,0 0,0 0,1 0,0 0,0 0,5 9,-4-12,0-1,0 1,0-1,1 1,0-1,-1 0,1 0,0-1,0 1,0-1,1 0,-1 0,1 0,-1-1,1 0,8 2,9 0,0 0,28-1,-37-2,28 2,-12 0,-1-1,1-1,0-2,40-7,-65 7,0 0,0 0,0 0,0 0,0-1,-1 1,1-1,-1 0,1 0,-1 0,0-1,0 1,0-1,-1 0,1 1,3-9,-4 8,0 0,-1 0,1 0,-1 0,0 0,0 0,0 0,0-1,-1 1,0 0,0 0,0-1,0 1,-1 0,0 0,1 0,-1-1,-2-3,0 4,0 1,0 0,0 0,0 0,-1 1,1-1,-1 1,1 0,-1 0,0 0,0 0,0 1,0 0,0-1,-6 0,-4-2,-28-9,-1 2,0 1,-1 3,-67-3,79 9</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3327 370,'-4'-1,"0"0,0 0,0 0,1 0,-1 0,0-1,1 0,-5-2,-9-5,8 6,-2-2,1 1,-2 0,1 0,0 1,-1 1,-13-2,22 4,-1 1,1-1,-1 0,1 1,-1 0,1 0,-1 0,1 0,0 0,0 1,-1 0,1 0,0-1,0 2,1-1,-1 0,0 0,1 1,-1 0,1-1,0 1,0 0,0 0,-3 6,1 1,0-1,0 1,1-1,0 1,0 0,1 0,-1 16,2 72,2-88,-2-6,1 0,0-1,1 1,-1 0,1 0,0-1,-1 1,2 0,-1-1,0 1,1-1,-1 0,1 1,0-1,0 0,0 0,1 0,-1 0,1 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1-1,1 0,-1 1,1-1,-1 0,5 0,30 4,0-2,0-1,50-4,-31 1,-47 0,15 2,-1-2,1-1,-1-1,43-10,-62 11,0 1,0-1,0 0,0-1,0 1,0-1,-1 0,0 0,1 0,-1 0,0-1,-1 0,1 0,-1 0,1 0,-1-1,0 1,-1-1,1 0,-1 1,0-1,0 0,-1 0,1-1,-1 1,0 0,0-11,0 9,-1 0,0 0,0 0,-1 0,0 0,0 0,0 0,-4-9,3 12,-1 0,1 0,0 0,-1 0,0 0,0 1,0 0,-1-1,1 1,-1 1,1-1,-1 0,0 1,-6-3,-29-14,-1 2,-1 1,-51-11,-134-17,190 38,-1 2,0 2,0 1,0 2,0 1,1 2,-1 2,1 1,-48 17,15 5</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink312.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:26:11.679"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 825,'-1'3,"1"6,0 3,4 5,8-1,9 0,2 1,7 5,5 2,5 1,3 3,0 1,1-2,-4-1,-5-5,-8-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">340 656,'0'3,"-4"2,-1 3,-7 8,-5 4,0 10,0 7,-4 8,-3 3,-1-2,4-3,2-7,5-8,4-3,7-8,8-5,7-6,1-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">594 677,'0'3,"0"9,0 13,0 9,3 10,2 9,3 1,0 3,3-1,-1-6,2-9,-2-6,-2-7,1-8,3-7,2-6,0-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">953 656,'-1'0,"0"1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 2,-10 24,10-25,-17 55,3 1,3 0,-9 118,20-174,0 1,0 0,0 0,0 0,1-1,-1 1,1 0,-1 0,1-1,0 1,0 0,0-1,1 1,-1-1,0 1,1-1,0 0,0 0,-1 0,4 3,-1-3,0 0,0 1,1-1,-1-1,1 1,0-1,-1 1,1-2,0 1,-1 0,7-1,31 3,80-5,-107 1,0-1,0 0,-1-2,1 1,-1-2,0 0,0 0,24-15,-33 17,-1-1,0 1,0-1,0 0,0 0,-1-1,0 1,0-1,0 1,0-1,-1 0,1 0,-1 0,-1-1,1 1,-1 0,1-7,0 0,-1 0,-1 1,0-1,-1 1,0-1,0 0,-5-14,4 20,-1 0,1 0,-1 1,-1-1,1 1,-1-1,1 1,-2 1,1-1,0 0,-1 1,-5-4,-3-2,-1 0,0 1,-21-10,2 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1165 380,'36'-12,"-18"5,-82-5,-191-40,246 49,20 2,3 2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1229 105,'0'-2,"0"0,1 0,-1 1,1-1,-1 0,1 1,0-1,0 0,0 1,0-1,0 1,0-1,0 1,1 0,-1-1,0 1,3-1,30-21,-25 18,3-2,0 0,0 1,1 1,0 0,0 1,0 0,1 1,-1 0,1 1,0 1,0 0,26 2,-38 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 0,0 1,-1-1,1 1,-1-1,1 1,-1 0,2 2,-1 0,0 1,-1-1,1 1,-1-1,1 1,-1-1,-1 1,1 6,0-1,-1 1,-1-1,0 0,0 1,-1-1,0 0,-6 14,4-15,-1 0,0 0,-1 0,0-1,0 0,-1 0,0 0,0-1,-1 0,0-1,0 0,0 0,-1 0,0-1,0-1,-1 1,1-2,-12 4,34-9,0 1,0 0,0 1,0 0,22 4,85 18,-90-15,-1 2,0 1,-1 1,0 1,-1 2,42 27,-66-39,0 1,0-1,0 1,0 0,-1 0,1 0,-1 0,0 0,1 0,-1 1,-1-1,1 1,2 5,-4-7,0 0,0-1,0 1,0 0,0 0,-1-1,1 1,0 0,-1-1,1 1,-1 0,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,-2 0,-27 10,-1 0,0-2,0-2,-1-1,-65 4,72-9</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink313.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:26:11.685"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">261 22,'-4'0,"-4"0,-5 0,-4 0,-2-4,-2-1,-1 1,0 0,0 2,0 0,0 1,1 4,3 6,1 4,4 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink314.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink308.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -29941,7 +29970,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink315.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink309.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -29973,26 +30002,56 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8346.24">3436 710,'4'1,"1"1,-1 0,0 1,0-1,0 1,0 0,0 0,0 0,0 0,-1 1,5 5,-4-5,13 17,-1 1,0 0,-2 1,23 49,-16-29,30 54,65 184,-100-230,-2 0,-3 1,-1 1,-3 0,0 92,-7-120,-1 15,-6 55,5-84,0-1,0 0,-1 0,0 0,0 0,-1-1,-1 1,0-1,0 0,-10 12,2-7</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10459.11">4537 1367,'34'-9,"-8"1,106-24,-97 21,1 2,0 2,39-3,-32 9,-31 2,0-1,-1-1,1 1,0-2,14-3,-13 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11170.4">4664 1790,'3'0,"5"0,13 0,12 0,12 0,9 0,6 0,8 0,2 0,4 0,4 0,-4 0,-4 0,-3 0,-9 0,-8 0,-8 0,-12 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31960">7035 1557,'-540'16,"489"-14,-7 1,56-3,7 0,34 0,617 0,-712 0,26 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33098.58">7395 1155,'0'-2,"0"1,1-1,-1 1,1-1,-1 1,1 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0 0,2-2,25-17,-15 11,17-12,2 1,0 1,1 2,1 2,0 0,1 3,53-13,-77 22,1 1,0 0,0 1,0 0,0 1,0 1,0-1,0 2,-1 0,1 0,13 5,-17-4,-1 0,0 1,0 0,0 0,0 0,-1 1,0 0,0 1,0-1,-1 1,1 0,-1 0,-1 1,1 0,-1-1,0 2,4 12,-2-6,-1 1,-1 0,-1 0,0 0,-1 1,0-1,-1 1,-1 0,-1-1,0 1,-1-1,0 1,-1-1,-1 0,-1 0,0 0,-1-1,0 0,-1 0,-1 0,0-1,-1 0,0-1,-1 0,0 0,-22 18,17-18,0 0,0-1,-2 0,1-1,-1-1,0-1,-1 0,0-1,0-1,-28 5,87-15,0 1,68 5,-90 0,1 0,-1 1,0 2,0 0,0 0,0 2,29 15,-41-19,-1 2,1-1,-1 1,0 0,-1 0,1 1,-1 0,0 0,0 0,-1 0,1 1,-2 0,1 0,3 9,-3-5,-1 0,-1 0,0 0,0 0,-1 0,-1 0,0 0,0 0,-3 15,3-22,-1-1,0 1,0 0,0-1,-1 1,1-1,-1 1,0-1,0 0,0 0,0 0,0 0,-1 0,-4 4,2-3,-1 0,1 0,-1 0,0-1,-1 0,1 0,-10 2,-8 2,0-2,-1-1,-34 1,48-4,-477 3,476-5,2 1,1 0,0 0,0-1,0-1,0 0,0 0,0 0,-11-6,20 8,0 0,-1 0,1 0,-1 0,1 0,0-1,-1 1,1 0,-1 0,1-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1-1,0 1,0 0,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,0-1,0 1,1-1,-1 1,0-1,13-10,1 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34244.53">8707 1917,'0'-1,"0"0,1 0,-1 0,0 0,1 0,0 0,-1 0,1 1,-1-1,1 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,-1 0,1-1,0 1,0 0,1 0,-1 0,0 0,1 0,30 0,-30 1,0 0,-1-1,1 1,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 1,-1-1,0 0,0 1,0-1,0 0,-1 1,1 0,0-1,-1 1,1-1,0 1,-1 0,0-1,1 1,-1 0,0 0,0-1,0 1,0 0,-1 2,1-1,-1 0,0 0,1 0,-1 0,0 0,-1 0,1-1,0 1,-1 0,0-1,1 1,-1-1,0 0,0 1,0-1,-1 0,-3 2,0 0,-1-1,0 0,0 0,0-1,0 0,-1 0,1-1,-1 1,1-2,-1 1,1-1,-1 0,1-1,-1 0,1 0,-1-1,1 1,0-2,0 1,0-1,0 0,-11-7,-4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34878.05">9046 1070,'0'11,"7"21,9 27,7 22,5 18,2 10,4 2,-2-4,-1-13,-3-12,-3-20,-5-16,-3-17,-1-13,1-12,-2-12,-4-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35949.25">9808 1007,'-24'0,"0"1,1 1,0 2,0 0,-30 10,49-13,-1 1,1 0,0 0,0 1,0-1,0 1,0 0,1 0,-1 0,1 1,0-1,0 1,0-1,0 1,0 0,1 1,-2 4,-2 5,1 1,1 0,-4 29,1-4,6-35,0-1,0 0,1 0,-1 1,1-1,0 0,2 8,-2-11,0 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1-1,1 1,0 0,0 0,0-1,0 1,-1 0,1-1,0 1,0-1,0 1,0-1,0 0,0 1,0-1,1 0,-1 0,0 0,0 1,0-1,0 0,0-1,0 1,0 0,0 0,2-1,65-15,-50 11,-1 1,1 0,26-1,-37 5,-1 0,0 0,1 1,-1 0,0 0,0 0,1 1,-1 0,-1 1,1-1,0 1,0 0,9 7,0 2,-2 1,0 0,0 1,-1 0,-1 1,16 26,-4 0,24 60,-40-86,-1 1,-1 0,0-1,0 2,-2-1,0 0,-1 1,-1 0,-1 32,-1-46,0-1,1 1,-1 0,-1-1,1 1,0-1,-1 1,1-1,-1 0,0 0,0 0,1 0,-1 0,-1 0,1 0,0-1,0 1,-1-1,1 1,-1-1,1 0,-1 0,0 0,-4 1,-9 2,0-1,0-1,-20 1,6-1,-17 4,21-4,0 1,0 1,0 2,-46 16,60-16</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37678.18">10845 986,'2'-2,"1"0,0 1,0 0,0 0,0-1,0 2,0-1,1 0,-1 1,0-1,0 1,0 0,1 0,-1 0,4 1,-5 0,0 0,0 0,0 0,-1 0,1 0,0 1,-1-1,1 0,-1 1,0-1,1 1,-1 0,0-1,0 1,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,1 0,-1 2,1 13,0 1,-1 0,-1-1,0 1,-2-1,0 1,-1-1,0 0,-2 0,0-1,-1 1,-11 19,-5 4,-1-1,-3-1,-46 53,55-70,0 0,-1-2,-2-1,1 0,-2-1,0-2,-38 20,60-35,-1 0,0 1,0-1,1 0,-1 0,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,0 1,1-1,-1 1,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 2,21 0,-10-1,25 1,0 2,-1 1,1 2,-2 1,1 2,-1 2,-1 0,0 2,0 2,50 34,-62-37</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38416.96">11289 922,'-22'68,"4"1,2 1,4 1,3 0,2 1,4-1,7 83,-1-122,2-1,1 1,1-1,1 0,2-1,1 0,1 0,2-2,29 47,-38-68,1-1,-1 1,2-1,-1 0,1-1,-1 1,2-1,-1 0,0-1,1 0,14 6,-19-9,1 0,-1 0,1 0,0-1,-1 1,1-1,-1 0,1 0,0 0,-1 0,1-1,0 1,-1-1,1 0,-1 0,1 0,-1-1,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,-1-1,1 1,-1-1,1 0,3-5,6-11,-1-1,0 0,-2-1,0 0,-1 0,-1-1,-2 0,0 0,4-41,-9 60,0 1,0-1,0 1,0 0,-1-1,1 1,-1-1,1 1,-1 0,0 0,0-1,0 1,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 1,-2-4,0 3,1 1,0-1,-1 0,1 1,-1 0,1 0,-1 0,1 0,-1 0,0 1,1 0,-5 0,-8 0,0 2,1 0,-1 1,1 1,-18 6,17-4,1 0,0 2,1-1,0 2,0 0,0 1,1 0,-18 19,16-13,0 1,1 1,1 1,0 0,-17 35,28-48,-1-1,1 1,0 0,0 0,0 0,1 0,0 7,1 4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39350.32">12157 1324,'-1'3,"9"13,9 14,12 19,16 21,12 11,6 8,7-2,2-4,0-9,-1-10,-10-12,-15-12,-15-16,-13-16,-10-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39744.76">12390 1388,'-4'10,"-4"16,-5 12,-4 9,-6 9,1 7,1 3,-1-6,5-2,1-8,3-9,1-10,1-8,7-8,8-6,10-5,3-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40212.9">12856 1134,'-1'10,"1"16,0 12,0 16,0 15,0 12,4 9,1 0,3 0,0-9,3-11,3-10,2-15,3-16,1-12,-3-13,-3-7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40937.81">13152 1240,'-10'177,"4"-113,5 125,2-180,0 1,1-1,0 1,0-1,1 0,0 0,1 0,0 0,0 0,1-1,0 0,1 0,0 0,0-1,0 1,1-2,0 1,0-1,1 0,0 0,0-1,0 0,1 0,-1-1,1-1,0 1,1-1,-1-1,0 1,1-2,-1 1,1-1,0-1,-1 0,1 0,13-3,-17 2,-1-1,1 1,-1-1,1-1,-1 1,0-1,0 0,0 0,0 0,0-1,-1 1,7-7,-4 1,-1 1,1-1,-1 0,-1 0,0 0,6-14,-2-3,0-1,-2 0,-1-1,3-37,-7 47,0 0,-2-30,-1 42,1 1,-1-1,-1 1,1-1,-1 1,0 0,0 0,0 0,-1 0,1 0,-1 0,-7-8,-18-14,-1 2,-2 1,0 1,-41-22,46 28,15 10,-38-21,47 27,0 0,-1 0,1 0,0 0,-1 1,1-1,-1 1,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-4 2,-4 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41827.78">13406 795,'-45'-1,"20"0,0 1,0 1,-42 7,187-47,-120 40,0-1,1 0,-1 0,1 0,-1 0,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,0-1,1 1,-1 0,0-1,0 1,1 0,-1 0,0-1,0 1,0-1,1 1,-1 0,0-1,0 1,0 0,0-2,-15 0,-28 4,27 3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="45681.59">13872 372,'-1'3,"1"6,-3 3,-2 9,-3 6,-1 7,2 4,2 7,1 3,2 0,1 0,1-6,0-5,0-6,1-8</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="46439.83">13787 562,'-63'2,"39"-1,-1 0,0-1,0-2,-29-5,52 7,-1-1,1 0,-1 0,1-1,0 1,-1 0,1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,1 0,-1 0,1-1,0 1,0-1,0 1,0-1,0 1,1-1,-1 1,0-5,0-7,0-1,1 1,2-27,0 15,2-116,-3 117</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48340.97">7331 2827,'3'-2,"0"0,1 0,0 0,-1 1,1-1,0 1,0 0,0 1,0-1,0 1,5-1,6-1,108-11,171 3,-211 9,2332-3,-1319 7,1523-3,-2578 0,-19 1,-1-1,1-1,-1-1,27-5,-44 5,0 1,-1-1,1 0,0-1,-1 1,1 0,-1-1,0 0,0 0,0 0,0 0,-1 0,4-5,16-17,47-30,94-55,43-34,-193 132,-1 1,0-1,-1-1,0 0,13-22,36-77,-36 63,212-466,-26-14,174-388,-307 770,-53 111</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="49204.43">16158 118,'-148'347,"93"-205,-569 1528,624-1669,-11 30,1 0,-2 1,0-2,-2 1,-2-2,-25 38,35-61,-1 0,-1-1,1 0,0 0,-1-1,0 1,0-2,-1 1,1-1,-1-1,-12 3,7-1,-32 9,-1-3,-51 4,-103 0,136-10,-2424 68,-1791-62,2379-12,1861 2</inkml:trace>
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink316.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink31.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-05-30T14:57:41.881"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1096,'3073'0,"-2412"30,-636-28,-6-1,0 0,-1 2,1 0,0 1,-1 0,19 8,-36-12,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,0 1,1-1,-1 0,1 1,-1-1,0 0,1 1,-1-1,1 0,-1 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,1 1,-1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 1,0-1,-1 1,1 0,0-1,0 0,0 1,-1-1,1 1,0-1,0 0,-1 0,1 1,-1 0,-10 7,-1 0,0-1,-1-1,1 0,-1-1,0 0,-22 5,-5 4,-83 29</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1237.35">469 1553,'16'0,"-1"-2,1 0,0 0,-1 0,1-2,22-9,86-43,-77 33,174-81,-217 101,1 1,-1 1,0-1,1 0,0 1,0 0,0 0,-1 1,1-1,1 1,-2 0,7 0,-8 1,-1 0,2 0,-2 0,0 1,0-1,0 1,1-1,-1 1,-1-1,1 1,0-1,0 1,-1 0,1 0,-1 0,2 1,-2-1,0 0,0 1,0-1,0 0,-1 1,2 3,4 18,-2-1,0 1,-1 0,-1 27,-11 105,3-68,5-67,-5 103,-24 127,20-204</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2546.39">1598 2037</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4403.39">2314 1375,'-14'16,"1"0,1 0,1 2,1-1,-1 0,3 2,0 0,-7 22,-1 0,-6 16,2 1,2 0,3 0,4 2,2-1,2 2,5 96,2-155,0 0,1 1,-1-1,1 1,0 0,-1-1,2 1,-1-1,0 1,1-2,-1 1,0 0,1 1,0-1,-1 0,1 0,0 0,0-1,3 4,1-3,-2 0,1 0,-1-1,1 1,1 0,-2-1,1 0,0 0,10 0,7 0,-2-2,2-1,-1 0,23-5,-26 3,1-1,0-1,28-11,-42 15,1-1,-1 1,1-1,-1-1,0 1,0 0,-1 0,0-1,2-1,-2 1,-1-1,1 2,-1-2,1 0,3-7,-6 8,-1 0,1 0,-1 0,0 0,0 0,0 1,-1-1,0 0,1 0,-1 0,-1 0,0 0,0 1,1-1,-1 1,0-1,0 1,-1-1,1 1,-1 1,0-1,1 0,-2 0,-3-2,-9-8,-1-1,-1 3,-22-13,31 19,0 0,1 1,-2 1,1-1,0 3,-1-2,1 1,-1 0,-9 0,-3 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5752.48">2864 1476,'-19'22,"1"1,1 1,2 0,0 0,-18 44,-8 11,23-49,9-16,1-1,0 1,1 0,0 1,2 0,-8 29,13-42,0 0,0 1,1-1,-1 0,1 0,-1 0,1 0,0-1,1 1,-1 0,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,-1 1,1-1,0 1,0-1,0-1,0 1,1 0,-1 0,0 0,0-1,0 1,0-1,4 1,11 3,-1-1,1-1,21 1,-27-2,75 1,-62-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6385.49">3057 1426,'-5'0,"-6"9,-1 11,1 11,-2 13,-3 13,-5 4,-7 10,-7 2,0 0,2 2,8-4,8-10,5-6,11-13,5-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7480.49">3277 1604,'-10'22,"2"0,-1 0,-4 34,-5 9,9-38,-2 2,2 1,2-1,1 1,0 0,2 0,1 39,4-66,0 1,0 0,0-1,0 1,0 0,1-1,-1 0,1 0,1 0,-1 1,0-1,1 0,-1 0,1 0,0-2,0 2,0-1,1 1,-1-1,0 0,0 0,1 0,-1-1,1 1,1-1,-2 0,7 1,-6-1,-1-1,1 0,1 1,-2-1,1 0,0 0,-1 0,1 0,1-1,-2 1,1 0,0-1,-1-1,1 1,-1 0,1-1,0 0,-1 0,0 0,0 0,0 0,0 0,0-1,-1 0,2 2,-2-2,0 0,3-5,0-2,-1 1,-1-2,1 2,-1-2,-1 2,0-2,0-16,-5-80,0 52,4 48,-1 0,0-1,-1 2,0-1,0-1,0 2,-2-1,1 0,0 0,-1 1,0-1,0 0,-1 1,0 1,-1-1,-8-10,-10-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8891.49">3801 1604,'0'0,"0"0,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0-1,-1 1,1 0,0-1,0 1,0 0,0-1,-1 1,1 0,0-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1-1,-1 1,-14 5,-14 18,16-11,1-1,0 2,1-1,0 2,2 0,-1 1,2-1,-13 28,22-41,-1 1,1 0,0-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 0,0 0,1 1,-1-1,0 0,1-1,-1 1,2 1,9 3,0-1,-1 1,19 4,11 5,-26-5,-1 0,0 0,-2 1,1 0,-1 1,0 0,-1 2,0-1,-2 1,0 0,9 17,-12-19,-1-1,1 2,-2-1,0 1,-1-1,0 1,-1 0,0 0,-1 1,-1-2,0 2,0-1,-1 0,-1-1,-3 13,3-20,1-1,-1 0,1 0,-1 0,0-1,-1 1,1 0,-1-1,0 1,1-1,-1 0,0 1,0-1,0 0,0-1,-1 0,1 1,-1-1,1 0,0 0,-1 0,1 0,-1 0,0-1,-6 1,-12 0,1-1,-1 0,-25-5,30 4,7 0,-1 0,1-1,0 1,0-2,1 0,-2 0,2-1,0 0,-12-7,-2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9612.49">4957 968,'-15'5,"-8"5,-19 23,-46 40,-30 12,-19 10,4-4,12-13,21-15,27-22,27-19</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10249.49">4186 1045,'4'0,"7"0,10 0,13 17,2 15,2 14,3 13,0 5,-8-5,0 2,-1-6,-5-8,-3-11,-6-5,-1-6,6-16,-2-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10757.59">5122 968,'0'22,"0"20,0 20,0 8,0 1,-5 11,-1-6,0-6,-4 2,1-8,0-4,8-14,13-18,5-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11960.59">5645 1147,'0'0,"0"-1,0 1,0-1,0 1,0-1,0 1,-2-1,2 1,0-1,0 1,0-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1-1,0 1,-1 0,1-1,0 1,-1 0,1-1,-1 1,1 0,0-1,-1 1,1 0,-1 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,0 1,-1-1,1 0,0 1,-1-1,1 1,0-1,-1 1,-30 23,2 9,2 1,2 1,1 1,-32 67,48-85,1 0,0 1,2-1,0 1,1 0,1 0,1 0,1 1,1 0,1-1,0 0,8 35,-8-50,1 0,-1 0,1 0,0 0,0 0,2 0,-2 0,1-1,0 1,0-1,0 0,0 1,0-1,1 0,0-1,0 0,0 0,0 1,0-1,0 0,2-1,-2 1,0-1,1 0,8 1,10 1,-1-2,0 0,1-2,29-3,-20 1,-19 2,-1 0,1-1,-2 0,2-1,-2-1,2 1,-2-1,1-1,-2 0,21-12,-25 12,2-1,-2 1,-1 0,1-1,0 0,-1-1,0 1,-1-1,0 0,1 0,-2 1,0-2,0 0,-1 1,0-1,2-13,-1 2,-2-1,0 1,-1 0,-2 0,1 0,-2 0,-1 0,-1 1,0-1,-13-26,14 36,0 0,-2 0,0 1,1-1,-1 1,-2 1,2-1,-1 1,-1 1,0-1,0 0,-1 1,0 1,0 0,0 0,-1 0,0 1,0 0,0 2,0-1,-22-4,28 7,-1 0,1 0,-1 0,1 0,-2 0,2 1,-1 0,1 0,-1 0,0 0,1 1,-6 3,-14 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13395.59">6196 1197,'-3'30,"-1"1,-1 0,-3-1,-12 34,8-23,-9 25,13-44,0 1,1 0,1 1,2-1,1 1,1 0,1 32,1-53,0-1,0 1,1-1,-1-1,1 2,0-1,-1 0,1 0,0 1,0-1,0 0,1 0,-1 0,1 0,-1-1,1 0,-1 1,1 0,0-1,1 1,-1-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,1-1,0 1,0-1,-1 0,0 0,1 0,-1 0,1-1,2 0,3 0,-1 0,0-1,1 0,-2 0,1-1,0 0,0 0,-1 1,0-2,0 0,1 0,4-6,-3 2,0-1,-1 0,-1-1,0 0,1 0,-2-1,-1 2,0-3,0 1,4-21,0-11,1-62,-7 79,-1 1,-2 0,-4-34,4 53,0 1,0-1,0 0,-1 1,0 0,0 0,0-1,-1 1,-1 0,1 1,0-1,-1 0,1 1,-1-1,0 1,-1 1,0-1,1 0,-1 1,0 0,-7-4,-10 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14169.59">6939 1147,'9'0,"8"0,6 0,3 0,12-4,8-2,11 0,19 1,20 3,44 0,9 1,-16 0,-26 1,-33 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15107.59">6718 1375,'1099'0,"-998"5,1 4,-1 3,142 36,-183-34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31543.89">12609 994,'-5'13,"-20"17,-14 12,-16 17,-22 24,-7 6,7-3,11-12,8-14,13-13,9-10,12-12</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32777.17">12032 739,'-17'1,"1"0,-1 0,1 1,0 1,0 1,0-1,0 2,1 1,0 0,0 1,-20 12,29-15,0-1,0 1,1 0,0 1,0 0,0 0,1-1,0 2,0 0,0-1,1 0,-1 2,1-1,0 0,1 0,0 0,1 1,-1 0,1-2,0 2,1 0,0 0,0-1,0 1,1-1,0 1,0-1,4 12,-3-14,0 1,1 0,0 0,0 0,0-1,0 0,1 1,-1-1,1 0,1 0,-1-1,0 0,0 1,1-1,10 5,-4-3,1 0,0-1,0 0,0 0,1-1,13 2,-23-5,0 0,0-1,0 1,0 0,0-1,0 0,1 0,-1 0,-1 0,1 0,0 0,-1-1,1 1,0-1,-1 0,1 0,0 0,-1 0,0 0,0 1,0-2,-1 1,1 0,0-1,-1 0,0 1,2-6,5-5,-2-2,-1 0,7-25,-5-2,-2 1,-2 0,-4-61,0 75</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34704.17">12638 1476,'-6'1,"2"0,0 0,0 0,-1 1,1-1,-1 1,1 0,0 0,1 0,-1 0,0 1,0-1,1 1,0 0,0 0,0 0,0 0,0 1,-2 4,-10 12,2 1,-11 26,14-30,-2 7,-53 107,58-114,0 1,1 1,1-1,2 0,-3 28,6-42,0 0,1-1,-1 1,1 0,0-2,0 2,0-1,0 1,1-1,0 0,-1 1,1-1,0-1,1 1,0 0,-1 0,1-1,-1 1,1-1,0 1,0-1,0 0,1-1,-1 0,1 1,-1 0,1-1,6 2,2 0,-1 0,1 0,0-2,0 1,0-1,0-1,0 0,14-2,-22 1,1-1,0 1,-1-1,-1 0,1 0,0 0,0-1,0 1,0-1,-1 1,0-1,0 0,0-1,0 1,-1-1,2 1,-2-1,0 1,0-1,2-4,4-11,1 1,7-35,-8 14,-3 1,-1-1,-3 1,-4-65,-1 5,5 92,0 1,-1-2,-1 1,1-1,-1 2,0-2,0 1,-1 0,0 1,0-1,-1 0,1 0,-1 0,0 1,-1 0,1-1,-1 1,-9-7,-2 2</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink310.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30030,7 +30089,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink317.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink311.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30057,7 +30116,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink318.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink312.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30095,7 +30154,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink319.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink313.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30119,6 +30178,177 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 23,'3'0,"6"0,4 0,10-4,6-1,8 1,6 0,2 2,0 0,1 1,-5 1,-5 0,-13 0,-13 0,-13 0,-12 0,-4 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink314.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:13.989"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'10'0,"12"0,12 0,12 0,4 0,5 0,1 0,-7 0,-3 0,-7 0,-5 0,-10 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink315.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:35.346"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 470,'3'0,"5"0,5 0,4 0,2 0,2 0,-7 0,-9 0,-8 0,-2 0,5 0,6 0,5-4,5-1,3 1,2 0,0 2,-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1158.74">339 68,'10'-2,"1"1,-1-1,1-1,-1 0,0-1,18-8,25-8,-53 20,74-17,-67 16,-1 0,1 0,-1 1,1 0,0 0,-1 1,1-1,-1 1,9 3,-13-3,0 1,1-1,-1 1,-1-1,1 1,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,-1-1,1 1,-1-1,1 5,0 6,0 0,-2 24,0-28,0 0,-1 1,0-1,0 0,-1 0,0 0,-1 0,0-1,0 1,-1-1,-9 13,-4 0,0-1,-36 30,2-2,41-33,11-14,0-1,1 0,-1 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,36-3,-24 1,-2 1,-1-1,1 1,0 1,-1 0,20 2,-27-2,-1 1,1 0,0-1,-1 1,1 0,-1 1,1-1,-1 0,1 1,-1-1,0 1,0 0,0 0,0-1,0 2,0-1,-1 0,1 0,-1 0,1 1,-1-1,0 1,2 4,0 7,0 0,-1 0,-1 1,0-1,-1 1,-1-1,-4 27,4-38,0 0,0 0,0 0,0 0,-1 0,0 0,1 0,-1-1,0 1,0-1,0 1,-1-1,1 0,-1 1,1-2,-1 1,0 0,1 0,-1-1,0 1,0-1,0 0,-1 0,1 0,0 0,-5 0,-11 2,0-1,1 0,-25-2,37 0,-13 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink316.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:46.176"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">62 724,'-1'3,"-2"2,-5 0,-5-2,-4 3,5 1,5-5,6-3,8-8,5-3,2-3,1 1,2 11,2 8,1 12,-3 9,-4 4,-4-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1616.09">401 194,'-1'0,"1"0,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 0,0 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1-1,23-8,-16 6,77-23,-75 23,0 1,0 1,0-1,1 2,-1-1,16 3,-24-2,0 1,0-1,-1 1,1-1,0 1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 1,0-1,1 1,0 1,0 2,0-1,-1 0,1 1,-1-1,0 1,0-1,1 9,-1-1,-1 0,0 0,-1 0,-1 0,-3 16,4-23,-1 0,0 0,0 0,0 0,-1 0,0-1,1 1,-2-1,1 1,0-1,-1 0,0 0,0-1,0 1,-5 2,-5 3,0-2,-1 0,-25 9,36-15,60 24,-46-17,1 1,-1 0,-1 1,1-1,-2 2,1-1,-1 1,-1 1,0-1,-1 1,0 0,-1 1,0-1,-1 1,0 0,-1 0,-1 1,0-1,-1 0,0 1,-2 20,1-31,0 0,-1-1,1 1,-1 0,1-1,-1 1,0 0,0-1,0 0,-1 1,1-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,-1-1,1 1,0 0,0-1,-4 2,-1 0,1-1,-1 0,0-1,0 0,0 0,0 0,0-1,-7 0,-5-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3341.38">951 110,'0'-5,"1"1,0 0,1-1,-1 1,1 0,0 0,0 0,0 0,1 0,-1 1,1-1,4-4,39-37,-46 44,1 1,-1-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,-1-1,1 1,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,-1 0,1 0,1 1,-1 0,0 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,0 1,2 11,-1 0,-2 23,1-30,-7 77,-4-1,-4 1,-42 135,55-214,1 0,-1 0,1 0,0 1,1-1,-1 0,1 1,0-1,1 7,-1-11,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,1 0,0 0,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 0,1 0,-1 0,0 0,5-1,28-10,-20 5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3953.75">1502 4,'-1'7,"1"6,1 12,-1 15,-1 16,1 10,1 6,-1 7,-1 4,1-5,1-5,-1-11,-1-9,1-10,1-13</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5331.1">1946 597,'4'5,"0"0,0 1,-1 0,6 11,3 5,65 110,59 90,-135-221,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,-1 1,1 0,0 0,0-1,0 1,0-1,0 1,0-1,0 1,1-1,0 1,-1-2,-1 1,1 0,0 0,-1 0,1-1,-1 1,1 0,0-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 1,-1-1,0 0,1 1,-1-1,0 1,1-2,2-5,-1 0,0 0,-1 0,2-13,5-154,-8 155,0-50</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5756.94">2221 321,'-4'0,"-4"3,-2 6,-1 11,-4 10,-2 14,-6 10,-6 4,-1 2,4 2,2 1,3-2,1-2,3-7,2-8,-1-12,6-15,5-11</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6207.91">2454 110,'0'7,"3"9,2 17,-1 17,0 15,2 17,1 13,2 12,4 6,2-6,3-13,-2-20,-3-22</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7296.46">2856 46,'-2'0,"0"0,0 1,0 0,0-1,0 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,0 0,0-1,0 1,0 0,0 0,-1 3,-16 53,15-47,-13 56,3 0,3 1,2 0,4 1,9 129,-5-195,1 0,-1 0,1 0,0 0,-1 0,2 0,-1-1,0 1,0 0,1 0,0-1,-1 1,1-1,0 0,0 1,0-1,1 0,-1 0,0 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,6 0,-4-1,0 1,0-1,1 0,-1 0,0-1,1 0,-1 0,0 0,0 0,0-1,0 0,0 0,0 0,-1-1,1 0,-1 0,6-4,-3-1,0 0,-1 0,0 0,0 0,-1-1,0 0,-1-1,0 1,0-1,-1 1,0-1,-1 0,2-14,0-17,-1 1,-3-42,-1 51,1-8,1 9,-8-60,5 79,0 1,-1-1,0 1,0 0,-2 0,1 1,-1-1,0 1,-10-13,13 20,-3-6,-1 0,0 1,-1 0,1 0,-1 1,-14-11,6 10</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink317.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:54.390"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">83 278,'-4'0,"-4"0,-5 0,0-4,-2-1,-1-3,6-1,7 2,8 1,7 3,5 1,4-2,1-1,-3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1082.78">464 2,'-55'-1,"-59"2,111 0,0 0,0 0,0 1,0-1,0 0,0 1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,0-1,1 1,0 0,-1 0,1 0,0 1,-1 3,2-5,-1 0,0 0,1 0,-1 0,1 1,0-1,-1 0,1 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,0 0,0 0,-1 0,1-1,1 1,-1 0,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 0,-1 1,1-1,0 0,0 0,0 0,0-1,4 2,9 0,0 0,1-1,-1-1,23-3,34 2,-69 1,-1 0,1 0,-1 1,0 0,1-1,-1 1,0 0,1 0,-1 0,0 1,0-1,0 0,0 1,0-1,0 1,0 0,2 2,-2 0,1 0,-1 0,1 1,-1-1,0 0,-1 1,1 0,1 6,-1 3,0 0,-1 0,-1 1,0-1,-2 16,1-26,-1-1,1 1,-1 0,1-1,-1 0,0 1,-1-1,1 0,0 0,-1 0,0 0,0 0,0-1,0 0,0 1,0-1,0 0,-1 0,1-1,-1 1,-4 1,-5 2,1-1,-1 0,-1-1,-24 4,-4-5,24-3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink318.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:57.785"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1287,'6'-5,"0"0,1 1,0 0,0 0,0 1,1 0,-1 0,1 1,13-3,-8 2,60-15,111-11,80 8,-233 19,1193-18,-885 22,9 0,511-3,-388-32,-338 15,201-56,-330 73,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,0 1,0-1,-1 0,1 1,-1-1,0 0,0-1,0 1,0 0,-1-1,1 1,-1-1,1-4,1-7,-1 1,-1 0,0-1,-2-26,-1 9,-3-63,-23-120,14 124,-5-153,20 73,0 148</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink319.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:33:01.016"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1543,'424'-28,"-130"4,183 9,175-12,-470 11,279-60,-449 73,1 0,-1-1,0 0,0-1,0 0,14-9,-19 9,-1 0,1-1,-1 0,-1 0,1 0,-1-1,0 1,-1-1,1-1,5-13,300-749,-229 552,-54 133,-18 56,0-1,2 2,17-34,-19 48</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -30169,177 +30399,6 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:13.989"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'10'0,"12"0,12 0,12 0,4 0,5 0,1 0,-7 0,-3 0,-7 0,-5 0,-10 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink321.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:35.346"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 470,'3'0,"5"0,5 0,4 0,2 0,2 0,-7 0,-9 0,-8 0,-2 0,5 0,6 0,5-4,5-1,3 1,2 0,0 2,-2 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1158.74">339 68,'10'-2,"1"1,-1-1,1-1,-1 0,0-1,18-8,25-8,-53 20,74-17,-67 16,-1 0,1 0,-1 1,1 0,0 0,-1 1,1-1,-1 1,9 3,-13-3,0 1,1-1,-1 1,-1-1,1 1,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,-1-1,1 1,-1-1,1 5,0 6,0 0,-2 24,0-28,0 0,-1 1,0-1,0 0,-1 0,0 0,-1 0,0-1,0 1,-1-1,-9 13,-4 0,0-1,-36 30,2-2,41-33,11-14,0-1,1 0,-1 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,1 0,-1 1,0-1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,36-3,-24 1,-2 1,-1-1,1 1,0 1,-1 0,20 2,-27-2,-1 1,1 0,0-1,-1 1,1 0,-1 1,1-1,-1 0,1 1,-1-1,0 1,0 0,0 0,0-1,0 2,0-1,-1 0,1 0,-1 0,1 1,-1-1,0 1,2 4,0 7,0 0,-1 0,-1 1,0-1,-1 1,-1-1,-4 27,4-38,0 0,0 0,0 0,0 0,-1 0,0 0,1 0,-1-1,0 1,0-1,0 1,-1-1,1 0,-1 1,1-2,-1 1,0 0,1 0,-1-1,0 1,0-1,0 0,-1 0,1 0,0 0,-5 0,-11 2,0-1,1 0,-25-2,37 0,-13 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink322.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:46.176"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">62 724,'-1'3,"-2"2,-5 0,-5-2,-4 3,5 1,5-5,6-3,8-8,5-3,2-3,1 1,2 11,2 8,1 12,-3 9,-4 4,-4-2</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1616.09">401 194,'-1'0,"1"0,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,1 1,-1-1,0 0,0 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1-1,23-8,-16 6,77-23,-75 23,0 1,0 1,0-1,1 2,-1-1,16 3,-24-2,0 1,0-1,-1 1,1-1,0 1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,0 0,1 1,-1-1,0 1,0-1,1 1,0 1,0 2,0-1,-1 0,1 1,-1-1,0 1,0-1,1 9,-1-1,-1 0,0 0,-1 0,-1 0,-3 16,4-23,-1 0,0 0,0 0,0 0,-1 0,0-1,1 1,-2-1,1 1,0-1,-1 0,0 0,0-1,0 1,-5 2,-5 3,0-2,-1 0,-25 9,36-15,60 24,-46-17,1 1,-1 0,-1 1,1-1,-2 2,1-1,-1 1,-1 1,0-1,-1 1,0 0,-1 1,0-1,-1 1,0 0,-1 0,-1 1,0-1,-1 0,0 1,-2 20,1-31,0 0,-1-1,1 1,-1 0,1-1,-1 1,0 0,0-1,0 0,-1 1,1-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,-1-1,1 1,0 0,0-1,-4 2,-1 0,1-1,-1 0,0-1,0 0,0 0,0 0,0-1,-7 0,-5-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3341.38">951 110,'0'-5,"1"1,0 0,1-1,-1 1,1 0,0 0,0 0,0 0,1 0,-1 1,1-1,4-4,39-37,-46 44,1 1,-1-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 1,-1-1,1 1,0 0,-1-1,1 1,0 0,0 0,0 0,-1-1,1 1,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,-1 0,1 0,1 1,-1 0,0 0,0 0,0 1,0-1,0 0,-1 1,1-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,0 1,2 11,-1 0,-2 23,1-30,-7 77,-4-1,-4 1,-42 135,55-214,1 0,-1 0,1 0,0 1,1-1,-1 0,1 1,0-1,1 7,-1-11,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,1 0,0 0,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 0,1 0,-1 0,0 0,5-1,28-10,-20 5</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3953.75">1502 4,'-1'7,"1"6,1 12,-1 15,-1 16,1 10,1 6,-1 7,-1 4,1-5,1-5,-1-11,-1-9,1-10,1-13</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5331.1">1946 597,'4'5,"0"0,0 1,-1 0,6 11,3 5,65 110,59 90,-135-221,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,-1 1,1 0,0 0,0-1,0 1,0-1,0 1,0-1,0 1,1-1,0 1,-1-2,-1 1,1 0,0 0,-1 0,1-1,-1 1,1 0,0-1,-1 1,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 1,-1-1,0 0,1 1,-1-1,0 1,1-2,2-5,-1 0,0 0,-1 0,2-13,5-154,-8 155,0-50</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5756.94">2221 321,'-4'0,"-4"3,-2 6,-1 11,-4 10,-2 14,-6 10,-6 4,-1 2,4 2,2 1,3-2,1-2,3-7,2-8,-1-12,6-15,5-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6207.91">2454 110,'0'7,"3"9,2 17,-1 17,0 15,2 17,1 13,2 12,4 6,2-6,3-13,-2-20,-3-22</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7296.46">2856 46,'-2'0,"0"0,0 1,0 0,0-1,0 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 1,0 0,0-1,0 1,0 0,0 0,-1 3,-16 53,15-47,-13 56,3 0,3 1,2 0,4 1,9 129,-5-195,1 0,-1 0,1 0,0 0,-1 0,2 0,-1-1,0 1,0 0,1 0,0-1,-1 1,1-1,0 0,0 1,0-1,1 0,-1 0,0 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,6 0,-4-1,0 1,0-1,1 0,-1 0,0-1,1 0,-1 0,0 0,0 0,0-1,0 0,0 0,0 0,-1-1,1 0,-1 0,6-4,-3-1,0 0,-1 0,0 0,0 0,-1-1,0 0,-1-1,0 1,0-1,-1 1,0-1,-1 0,2-14,0-17,-1 1,-3-42,-1 51,1-8,1 9,-8-60,5 79,0 1,-1-1,0 1,0 0,-2 0,1 1,-1-1,0 1,-10-13,13 20,-3-6,-1 0,0 1,-1 0,1 0,-1 1,-14-11,6 10</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink323.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:54.390"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">83 278,'-4'0,"-4"0,-5 0,0-4,-2-1,-1-3,6-1,7 2,8 1,7 3,5 1,4-2,1-1,-3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1082.78">464 2,'-55'-1,"-59"2,111 0,0 0,0 0,0 1,0-1,0 0,0 1,0 0,0 0,1 0,-1 0,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,0-1,1 1,0 0,-1 0,1 0,0 1,-1 3,2-5,-1 0,0 0,1 0,-1 0,1 1,0-1,-1 0,1 0,0 0,0 0,1 0,-1 0,0 1,1-1,-1 0,1 0,0 0,0 0,-1 0,1-1,1 1,-1 0,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 0,-1 1,1-1,0 0,0 0,0 0,0-1,4 2,9 0,0 0,1-1,-1-1,23-3,34 2,-69 1,-1 0,1 0,-1 1,0 0,1-1,-1 1,0 0,1 0,-1 0,0 1,0-1,0 0,0 1,0-1,0 1,0 0,2 2,-2 0,1 0,-1 0,1 1,-1-1,0 0,-1 1,1 0,1 6,-1 3,0 0,-1 0,-1 1,0-1,-2 16,1-26,-1-1,1 1,-1 0,1-1,-1 0,0 1,-1-1,1 0,0 0,-1 0,0 0,0 0,0-1,0 0,0 1,0-1,0 0,-1 0,1-1,-1 1,-4 1,-5 2,1-1,-1 0,-1-1,-24 4,-4-5,24-3</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink324.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:32:57.785"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1287,'6'-5,"0"0,1 1,0 0,0 0,0 1,1 0,-1 0,1 1,13-3,-8 2,60-15,111-11,80 8,-233 19,1193-18,-885 22,9 0,511-3,-388-32,-338 15,201-56,-330 73,-1 0,1 0,-1-1,1 1,-1-1,0 0,0 0,0 0,0 0,0-1,0 1,0-1,-1 0,1 1,-1-1,0 0,0-1,0 1,0 0,-1-1,1 1,-1-1,1-4,1-7,-1 1,-1 0,0-1,-2-26,-1 9,-3-63,-23-120,14 124,-5-153,20 73,0 148</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink325.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:33:01.016"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#E71224"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1543,'424'-28,"-130"4,183 9,175-12,-470 11,279-60,-449 73,1 0,-1-1,0 0,0-1,0 0,14-9,-19 9,-1 0,1-1,-1 0,-1 0,1 0,-1-1,0 1,-1-1,1-1,5-13,300-749,-229 552,-54 133,-18 56,0-1,2 2,17-34,-19 48</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink326.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:33:05.440"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -30359,7 +30418,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink327.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink321.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30387,7 +30446,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink328.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink322.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30415,7 +30474,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink329.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink323.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30449,35 +30508,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink33.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-05-30T15:03:06.743"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-      <inkml:brushProperty name="color" value="#AB008B"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">111 0,'0'32,"0"37,-5 38,-5 33,-6 15,-5 8,1 35,4-8,5-26,5-33,2-34,3-28,1-23,0-13,1-9,5-4,0-4</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1748">1064 106,'-1'8,"-1"0,1 0,-1 0,0 0,-1-1,0 1,0-1,-7 12,0 0,-149 270,-9 19,156-280,1 0,1 1,2 0,1 0,1 1,-2 33,7 180,1-238,0 92,-2-57,3 0,9 66,-8-96,0-1,1 0,0 0,1 0,0 0,0 0,1-1,0 1,10 11,-13-18,0 1,0-1,1 1,-1-1,0 0,1 0,0 0,-1 0,1-1,0 1,0-1,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,0-1,1 0,-1 0,0 0,0 0,1 0,-1-1,0 0,0 1,0-1,0 0,5-3,14-10,-1-1,-1-1,0 0,-2-2,0 0,0-1,-2-1,27-42,-38 53,1-1,-1 0,-1 0,0 0,0 0,-1-1,0 1,-1-1,0 0,-1 0,0 0,-1 0,0 0,-1 0,0 0,-1 0,0 0,0 1,-1-1,-1 1,0-1,0 1,-1 0,0 1,-1-1,0 1,0 0,-1 1,0-1,-1 1,0 1,0-1,0 1,-1 1,0 0,-1 0,1 1,-1 0,0 0,0 1,-1 1,1-1,-1 2,-18-3,-52 5,58 1</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink330.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink324.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30505,7 +30536,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink331.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink325.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30532,7 +30563,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink332.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink326.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30562,7 +30593,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink333.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink327.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -30595,6 +30626,209 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink328.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T20:57:11.250"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">65 339,'-4'4,"0"1,1 0,0 0,0 0,0 0,1 1,0-1,-3 10,-8 50,10-46,-6 35,3 1,2 0,4 65,1-109,0-1,1 1,1-1,0 0,0 1,1-1,0-1,1 1,0-1,0 1,1-1,0-1,8 9,-8-10,0-1,0 0,0 0,1-1,0 0,0 0,0 0,1-1,-1 0,1-1,0 0,0 0,1 0,-1-1,0-1,14 2,-6-2,-2 0,1 0,0-1,0-1,0 0,-1-1,19-5,-28 4,0 0,-1 1,1-2,-1 1,1-1,-1 1,0-1,-1 0,1-1,-1 1,0 0,0-1,0 0,0 0,-1 0,0 0,3-9,0-3,0 0,-1-1,-1 0,1-21,-6-192,1 218,-2 0,1 0,-2 0,0 0,0 0,-1 1,-1 0,0 0,0 0,-1 1,-1 0,-17-20,17 21,-1 2,0-1,-1 1,1 0,-2 1,1 0,-1 1,0 0,0 0,0 2,-1-1,0 1,0 1,-12-2,3 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="898.3">891 953,'3'0,"5"0,-2 0,-2 3,-6 2,-6 3,-5 1,-1-6,3-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2160.5">1314 466,'-1'0,"0"0,0 1,0-1,0 0,0 1,0-1,1 1,-1-1,0 1,0-1,1 1,-1 0,0-1,1 1,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 1,-9 23,8-18,-7 15,2 1,1 0,0 0,2 1,1-1,0 1,2 0,1 0,1 0,0 0,2-1,1 1,1-1,1 0,1 0,1 0,1-1,1 0,1-1,1 0,0-1,2 0,0-1,20 20,0-5,1-1,2-2,1-1,1-2,2-2,0-1,68 28,-86-43,0-2,1-1,0 0,0-2,1-1,31 1,-52-5,0 0,0 0,-1-1,1 1,-1-1,1 0,0 0,-1-1,0 1,1-1,-1 0,0 1,0-1,0-1,0 1,0 0,0-1,0 0,-1 1,0-1,1 0,-1 0,0 0,-1-1,4-5,1-7,-1 0,0-1,-1 0,3-23,-3 16,3-17,-1-2,-3 1,-1-1,-2 1,-8-62,5 93,0 0,-1 0,0 0,0 1,-1-1,-1 1,0 1,0-1,-1 1,0 0,-1 0,0 1,0 0,-1 1,-17-13,2 5,0 0,0 2,-1 1,-1 1,-38-11,22 11,-1 2,-1 2,1 2,-1 2,0 2,-46 4,85-3,0 0,0 0,0 1,0 0,0 0,0 0,0 0,1 1,-1 0,1 0,-1 0,-7 6,4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3349.88">2436 339,'-3'0,"1"1,-1-1,1 1,0 0,-1 0,1 0,0 0,0 1,0-1,0 0,0 1,0 0,0-1,1 1,-1 0,1 0,-1 0,-2 4,-21 39,20-31,0 0,1 1,0-1,1 1,1 0,0 0,1 18,2 7,7 59,-7-94,1 11,0-1,1 0,10 29,-11-39,0-1,0 1,1 0,0-1,0 1,0-1,1 0,0 0,-1-1,1 1,0-1,1 0,-1 0,1 0,6 3,29 10,2-2,-1-2,2-1,52 5,-40-6,12 2,1-3,0-3,134-5,-198-1,-1 0,1-1,0 1,-1-1,1 0,-1 0,0 0,1 0,-1-1,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0-1,-1 1,0-1,1 0,-1 0,0 0,0 0,-1 0,1 0,-1 0,1-1,1-5,-1-5,0-1,0-1,-1 1,-1 0,-3-24,1-2,1 30,0 0,-1 0,-1 0,1 1,-2-1,1 1,-2-1,1 1,-1 1,-1-1,0 1,0-1,-1 2,0-1,0 1,-1 0,-14-11,-1 1,-1 1,0 1,-1 1,-1 2,-43-18,40 19,-1 2,-1 0,1 2,-1 1,-1 2,1 1,-39 0,-10 6,80-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4891.41">4193 234,'0'621,"1"-705,-3-96,1 177,0-1,1 1,-2-1,1 1,0 0,-1-1,1 1,-1 0,0 0,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,-1 0,1 0,-5 0,-12-4,0 2,-1 0,-32 1,38 1,-128 0,141 1,0 0,0-1,0 1,0-1,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,0 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 1,0-1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-4,-1-8,2 1,-1-1,3-24,0 15,-1-85,2-69,0 152,2 7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6367.5">4764 149,'-5'0,"0"0,0 0,1 0,-1 1,1 0,-1 0,0 0,1 1,0 0,-1-1,1 2,0-1,0 0,0 1,0 0,1-1,-1 2,1-1,-1 0,1 1,0-1,1 1,-4 5,1 1,0 0,1 1,0 0,1 0,0 0,1 0,0 0,0 18,1-12,-1-4,1 0,1-1,0 1,3 14,-3-24,1-1,-1 1,1 0,0-1,0 1,0-1,0 1,0-1,1 0,-1 1,0-1,1 0,0 0,0 0,0 0,0 0,0-1,0 1,0 0,0-1,1 0,-1 1,0-1,6 2,1-1,1 0,0 0,0-1,-1 0,1-1,0 0,0 0,0-1,16-4,-20 4,-1-1,1 0,-1 0,1 0,-1 0,0-1,0 0,0 0,0 0,-1-1,1 0,-1 1,0-2,0 1,0 0,-1-1,5-8,2-4,-2-1,0 0,-1 0,8-39,-13 53,-1-1,-1 0,1 1,-1-1,0 0,0 0,0 1,0-1,-1 0,0 1,0-1,0 0,-1 1,1-1,-1 1,0 0,-1 0,1-1,-1 1,1 1,-1-1,0 0,-1 1,1-1,-1 1,-5-4,-5 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6926.69">5484 1,'-55'46,"19"-5,2 1,2 2,2 1,2 1,-31 73,14-13,-46 169,88-264,0-2,0 0,1 0,0 1,0 11,1-19,1-1,0 1,0-1,0 1,0-1,1 1,-1-1,0 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1-1,0 1,0 0,1 0,-1-1,1 1,-1-1,3 1,13 1,-1 0,2-1,28-3,-19 1,21-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7576.75">5674 699,'-12'-1,"0"1,0 1,0 0,0 1,0 0,-12 4,20-5,0 1,1 0,-1 0,0 0,1 1,-1 0,1-1,0 1,0 0,0 0,0 1,0-1,1 1,0-1,-1 1,1 0,1 0,-1 0,0 0,0 5,-3 11,1 0,0 0,2 1,0-1,2 1,1 24,-1-43,0 0,0 0,1 1,-1-1,0 0,1 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,1 1,-1-1,1 1,2 1,-2-2,1-1,0 1,-1 0,1-1,-1 0,1 1,0-1,-1 0,1 0,-1-1,1 1,0 0,-1-1,1 0,3-1,6-3,1 0,-2-1,1-1,-1 0,0 0,10-10,-12 9,-1 0,-1-1,1 0,-1 0,-1 0,8-16,-11 20,0 0,-1 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0-1,-1 1,0 0,0-1,0 1,0 0,-3-11,2 14,0-1,0 1,-1-1,1 1,-1-1,0 1,1 0,-1 0,0-1,0 2,0-1,-1 0,1 0,0 1,-1-1,1 1,-1-1,0 1,-2-1,-3 0,0 0,-1 0,1 1,0 0,-11 0,1 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8593.38">23 2308,'14'-1,"1"0,0-2,25-5,16-4,730-56,11 53,-757 15,2694-1,-1153 4,-1564-3,-10 0,1 0,0 0,0 0,9-3,-15 2,0 1,1-1,-1 0,0 0,0 0,1 0,-1-1,0 1,0-1,0 1,-1-1,1 0,0 1,-1-1,1 0,-1 0,2-3,98-198,139-219,111-209,-281 482,66-119,-105 223,-19 34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9420.71">7219 488,'-1'12,"-1"0,0 0,0 0,-1 0,-1 0,-5 12,-1 6,-197 820,148-573,38-132,20-140,1-3,-1 1,0 0,1 0,-1-1,0 1,0-1,-1 1,1-1,-1 1,1-1,-1 0,0 0,1 1,-1-1,0-1,-1 1,1 0,-4 2,-4 2,-1 0,0-1,-14 4,-5 3,-24 11,-2-3,0-2,-1-3,0-2,-97 9,-298-9,353-13,-4356-3,4418 3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink329.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:00:40.337"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">270 89,'15'-2,"0"0,-1-1,1 0,0-1,-1-1,0 0,27-15,-23 12,0 0,0 1,0 0,22-3,-31 8,1 1,-1 0,1 1,-1 0,1 0,0 1,-1 0,1 1,-1 0,17 6,-21-6,-1 0,0 0,0 1,1 0,-1 0,-1 0,1 0,0 0,-1 1,0 0,0-1,0 1,0 1,0-1,-1 0,0 0,0 1,0 0,-1-1,1 1,-1 0,1 8,0 2,0 0,-1 0,-1 0,0 0,-3 16,2-26,0 0,0-1,0 1,0 0,-1-1,0 1,0-1,0 0,-1 0,1 1,-1-2,0 1,0 0,0 0,-1-1,1 0,-1 0,0 0,-5 4,-12 2,0-1,-1-1,1-1,-2 0,1-2,-33 3,36-2,19-5,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,39 7,-14-6,124 14,-134-13,-1 2,1-1,-1 2,0 0,0 1,-1 0,25 16,-35-20,0 1,0 0,0 0,-1 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,-1-1,0 1,0 0,0 0,-1 0,1 0,-1 6,0 9,0 0,-5 29,4-42,0-2,0 1,0-1,0 0,-1 0,1 0,-1 0,0-1,0 1,-1 0,1-1,-1 1,0-1,1 0,-2 0,1 0,0 0,0-1,-7 4,-5 3,-1-1,0-1,-21 7,7-3,-3 4,-1-2,-1-2,0 0,-1-3,-52 6,-16-8,-155-12,256 6,0 0,1 0,-1 0,0 0,1-1,-1 0,1 1,-1-1,1 0,-1 0,1 0,-1-1,1 1,0 0,0-1,-1 0,1 1,0-1,-1-2,0-5</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink33.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-05-30T15:03:06.743"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">111 0,'0'32,"0"37,-5 38,-5 33,-6 15,-5 8,1 35,4-8,5-26,5-33,2-34,3-28,1-23,0-13,1-9,5-4,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1748">1064 106,'-1'8,"-1"0,1 0,-1 0,0 0,-1-1,0 1,0-1,-7 12,0 0,-149 270,-9 19,156-280,1 0,1 1,2 0,1 0,1 1,-2 33,7 180,1-238,0 92,-2-57,3 0,9 66,-8-96,0-1,1 0,0 0,1 0,0 0,0 0,1-1,0 1,10 11,-13-18,0 1,0-1,1 1,-1-1,0 0,1 0,0 0,-1 0,1-1,0 1,0-1,0 1,0-1,0 0,0 0,1 0,-1-1,0 1,0-1,1 0,-1 0,0 0,0 0,1 0,-1-1,0 0,0 1,0-1,0 0,5-3,14-10,-1-1,-1-1,0 0,-2-2,0 0,0-1,-2-1,27-42,-38 53,1-1,-1 0,-1 0,0 0,0 0,-1-1,0 1,-1-1,0 0,-1 0,0 0,-1 0,0 0,-1 0,0 0,-1 0,0 0,0 1,-1-1,-1 1,0-1,0 1,-1 0,0 1,-1-1,0 1,0 0,-1 1,0-1,-1 1,0 1,0-1,0 1,-1 1,0 0,-1 0,1 1,-1 0,0 0,0 1,-1 1,1-1,-1 2,-18-3,-52 5,58 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink330.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:00:46.671"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2 1,'-2'179,"16"366,-13-536,-1-3,0 0,1 0,0 0,0 0,0 0,1 0,-1 0,2 0,-1-1,0 1,1-1,5 8,-8-13,1 0,-1 1,0-1,0 0,1 0,-1 0,0 1,0-1,1 0,-1 0,0 0,1 0,-1 1,0-1,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,0 0,1 0,-1-1,10-13,1-24,-10 35,15-56,29-71,-36 106,2 1,1 1,1-1,1 2,29-35,-35 48,0 0,1 1,0 1,0-1,1 2,0-1,0 1,0 1,0-1,1 2,0 0,0 0,0 1,18-2,-16 3,1 0,0 1,-1 1,1 0,0 1,-1 0,1 1,-1 0,0 1,0 1,21 10,-25-8,1-1,-1 1,0 0,-1 1,0 0,0 0,-1 1,1-1,-2 2,0-1,0 1,0 0,-2 0,1 1,-1-1,4 21,-1 0,-2 1,-1 0,-2 0,-2 53,-1-67</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="667.68">1124 276,'3'0,"5"0,5 0,4 0,2 0,2 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,-3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1222.68">1018 572,'3'0,"9"0,13 0,6 0,8 0,9-4,3-1,0 1,-2 0,-4-2,-8 0,-5 0,-6 2,-6 2</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink331.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:00:59.618"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">30 45,'4'-1,"1"0,-1-1,1 1,-1-1,8-4,6-1,-1 1,1 1,-1 1,1 0,0 1,0 1,0 1,0 1,0 0,31 6,-47-6,0 0,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1 0,-1 0,0-1,0 1,2 3,-3-1,1-1,-1 0,1 0,-1 0,0 0,0 0,0 1,-1-1,1 0,-1 0,1 0,-1 0,-2 4,0 2,-1-1,0 0,-1 0,0-1,0 1,-1-1,1 0,-1 0,-11 8,7-8,-1-1,0-1,0 1,0-2,-17 5,4 0,78-7,-34-3,-1 0,0 1,0 1,0 0,0 1,23 6,-38-6,1-1,-1 1,1 0,-1 0,0 0,0 0,0 1,0 0,0 0,0 0,-1 0,0 1,1-1,-1 1,-1 0,1 0,0 0,-1 0,0 0,0 1,0-1,-1 1,1-1,-1 1,0 0,0 6,2 8,-2 1,0 35,-2-49,1 0,-1 0,0 0,0-1,-1 1,0 0,0-1,0 1,0-1,-1 0,0 0,0 0,-7 8,0-4,0 0,-1-1,0 0,-1 0,0-1,0-1,0 0,-1-1,1 0,-1-1,-1-1,-20 4,-12-1,-1-3,-59-2,89-2,-15 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink332.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:01:04.545"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 103,'1'13,"0"0,2 0,-1 0,8 18,1 10,25 130,39 151,-68-291,-6-24,0 0,1 1,0-1,0 0,0 0,1 0,0 0,1-1,-1 1,6 6,1-8,-1-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1332.9">382 166,'-1'-10,"1"0,1-1,0 1,1 0,0 1,0-1,5-13,-4 18,-1 0,1 0,0 1,0-1,0 1,1 0,0 0,0 0,0 0,0 1,0 0,1-1,-1 2,1-1,7-3,-10 5,1 0,-1 0,0 0,0 0,1 1,-1-1,0 1,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1 1,-1-1,0 1,1-1,-1 1,0 0,3 1,-2 1,0-1,0 0,-1 1,1-1,-1 1,0 0,1 0,-1 0,-1 0,1 0,0 1,1 5,3 9,-2 1,0 0,-1 0,1 23,-4-40,2 34,-1-1,-4 44,1-61,-1 0,-1-1,-1 1,0-1,-1 0,-10 20,-30 39,20-34,24-40,1 0,0 0,0 1,-1-1,2 0,-1 1,0-1,0 0,0 6,1-8,1 1,-1 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 1,-1-1,1 1,-1-1,1 1,-1-1,0 1,1-1,0 1,-1-1,1 0,-1 1,1-1,-1 0,1 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1-1,1 1,0 0,0-1,22-4,-1-1,0-1,-1-1,32-17,20-7,-55 26</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink333.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:01:24.832"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'0'700,"0"-681</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="417.55">298 742,'3'0,"2"0</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink334.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -30609,7 +30843,7 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2021-06-04T23:34:22.782"/>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:01:27.118"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.1" units="cm"/>
@@ -30618,13 +30852,145 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">867 65,'0'10,"0"16,0 16,0 20,3 24,2 23,4 18,3 13,3 0,7-2,-1-6,0-12,-3-22,-6-20,-4-21,0-19,2-17,0-11</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="729.93">846 700,'-35'-1,"1"1,-1 2,1 2,0 1,-64 17,84-16,6-3,0 0,0-1,0 0,0 0,-15 1,21-3,1 0,-1 0,0 0,1 0,-1 0,1-1,-1 1,1-1,-1 1,1-1,-1 0,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 0,1 1,0-1,0 1,-1-1,1-1,-3-49,5-92,1 58,0-241,-3 290</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2145.17">1502 361,'1'-4,"0"1,0 0,1 0,-1 0,1 0,0 0,0 0,0 1,5-6,5-6,5-5,-6 12,-10 7,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 1,-1 0,1-1,0 1,0 0,0-1,0 1,-1-1,1 1,0 0,0-1,-1 1,1-1,0 1,-1 0,1-1,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,0-1,1 0,-1 0,0 1,0-1,-25 9,22-8,0 0,0 0,0 0,0-1,0 1,0-1,0 1,0-1,1-1,-1 1,-5-1,9 1,-1-1,1 1,-1 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,0 1,-1-1,1 1,0-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,0-1,0 1,-1-1,1 0,1-1,-1 0,0 0,1 0,-1 0,1 0,0 0,0 1,0-1,0 0,0 0,0 1,2-3,2-2,-1 1,1 0,0 0,1 0,10-7,-15 11,0 0,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 1,-1-1,1 1,0 0,0-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,2 12</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2691.18">2391 1,'-2'32,"-1"1,-10 39,2-6,-27 217,-3 457,41-738,0 13,1 1,3 20,1-18</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3546.12">2899 1102,'-3'2,"1"0,-1 0,0 0,1-1,-1 1,0-1,0 1,0-1,0 0,0 0,0-1,0 1,-1 0,1-1,0 0,0 0,0 0,-6-1,7 1,0 0,0-1,0 1,0-1,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 0,0 1,0-1,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1-2,1-5,1 0,-1 0,2 0,-1 0,1 1,0-1,1 1,0-1,0 1,1 0,0 0,8-11,8-10,41-47,-50 63,-3 4,25-28,-32 36,1-1,0 0,0 1,0-1,0 1,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 1,1-1,3 1,-4 0,-1 1,1-1,-1 1,0 0,1 0,-1 0,0-1,1 1,-1 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,-1 0,1 1,0-1,-1 1,1-1,-1 1,1-1,-1 1,0-1,0 1,1 2,2 50,-3-48,0 4,0 1,-1-1,0 0,-1 0,-3 11,5-19,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1-1,0 1,0-1,0 1,0-1,0 1,0-1,-1 0,1 1,0-1,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1-1,0 1,1-1,-1 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,1-1,-3 0,2 0,0 0,0 0,0 0,0-1,0 1,1 0,-1-1,0 0,1 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1-1,1 1,-1 0,1 0,0-5,-1 3,1 0,0 1,0-1,0 0,0 0,1 0,0 0,0 0,0 0,0 0,0 1,1-1,1-3,-2 6,-1 1,0 0,0-1,0 1,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,1-1,-1 1,0 0,1 0,-1 0,0-1,1 1,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 1,0-1,1 0,9 18,-1 22,-7-20</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212241.44">318 1695,'1106'16,"1395"10,-2495-26,1 0,-1 0,0 0,0-1,0 0,0 0,8-3,-12 2,1 1,-1-1,0 1,0-1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1-1,0 1,0-1,0 1,0-1,0 1,0-6,61-333,-26 113,52-171,-55 254,-32 141,6-31,2 0,25-62,-26 81</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="213128.68">4805 446,'-188'453,"-84"220,258-633,-7 14,2 0,4 1,-11 64,25-109,-1 1,0-1,-1 0,0 1,0-2,-6 14,6-19,1 0,0-1,-1 1,0 0,0-1,0 0,0 0,0 0,-1 0,1 0,-1-1,0 0,0 0,0 0,0 0,0 0,-8 1,-35 6,-1-2,0-2,-84-2,74-3,-1857 0,1873 0,-1053-62,910 40,-340-25,475 48,36 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2 786,'-1'-23,"0"8,1 1,1-1,0 0,4-18,-4 30,0 0,-1 0,1 0,0 1,1-1,-1 0,0 0,1 1,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,0 0,1 1,-1-1,1 1,0-1,-1 1,1 0,0 0,0 0,5 0,0-1,0 1,0 1,0-1,0 1,0 1,0-1,0 1,-1 1,1 0,0 0,13 5,-17-4,0-1,0 0,0 1,0 0,-1 0,1 1,-1-1,0 0,0 1,0 0,0 0,-1 0,1 0,-1 0,0 1,0-1,-1 0,1 1,-1 0,0-1,0 6,2 10,-1 0,-1 0,-1 1,-1-1,-1 0,-1 0,0 0,-2 0,0-1,-1 0,-1 0,0 0,-2-1,0 0,-1 0,-1-1,-1-1,-17 21,11-18,13-14,-1 1,1 0,0 0,0 1,1-1,-5 11,8-16,1-1,0 1,0 0,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,0 1,1-1,-1 1,0 0,1-1,0 1,19 7,32-8,-44 0,104-4,-94 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1369.81">510 765,'-1'-20,"1"1,1-1,2 1,7-35,-9 49,0 1,1-1,0 1,0 0,0-1,0 1,1 0,-1 1,1-1,0 0,0 1,1 0,-1-1,1 1,0 1,-1-1,1 0,0 1,1 0,-1 0,0 0,0 0,1 1,-1 0,1 0,5-1,-3 1,0 0,1 1,-1 0,0 0,1 0,-1 1,10 2,-14-2,0 0,0 0,0 0,0 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,0 1,0-1,0 1,0-1,-1 1,1 0,-1-1,3 6,1 6,15 34,22 82,-38-115,-1-1,-1 1,0 0,-1 0,-1 0,0-1,-1 1,0 0,-2 0,-5 23,2-27,1 1,-2-1,0-1,0 1,-1-1,-14 15,7-7,-5-1,17-15,1-1,-1 1,1 0,0 0,-1 0,1 0,0 1,0-1,0 1,1-1,-1 1,0 0,1-1,0 1,0 0,-2 5,3-7,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0-1,-1 1,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,0 0,0 0,0 0,2 0,44 2,-39-2,124-1,-107 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2672.35">1378 638,'-52'-2,"34"0,-1 2,0 0,1 1,-36 6,52-6,-1 0,1 1,-1-1,1 0,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,1 0,-1 0,1-1,-1 1,1 0,0 0,0 5,0-4,0 0,0 0,0 0,1 0,0 0,-1-1,1 1,1 0,-1 0,0-1,1 1,0-1,0 1,0-1,0 0,1 1,-1-1,1 0,5 4,-1-3,0 0,1-1,-1 0,1-1,0 0,-1 0,1 0,15 1,69-3,-62-1,-24 1,0-1,1 1,-1-1,0 0,0-1,0 0,0 0,-1 0,1 0,-1-1,1 0,-1 0,0 0,0-1,0 0,5-5,-5 3,0 0,0 0,0-1,-1 0,0 0,0-1,-1 1,0-1,0 1,-1-1,3-14,-2 6,-2-1,0 1,-1-22,1 164,4 79,0-164,2-1,13 48,-11-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3193.73">1928 743,'2'0,"0"1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,0-1,0 1,0 0,-1 0,3 3,2 2,11 9,196 191,-149-149,104 69,-118-92,2-3,0-2,97 39,-144-67,0 0,1-1,-1 1,1-1,-1-1,1 1,6-1,-10 0,-1 0,0 0,1 0,-1-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 0,1 0,0 0,0-1,-1 1,1 0,-1 0,1 0,-1-1,0 1,0 0,1 0,-1-1,0-1,0-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3638.39">2478 828,'-4'0,"-4"0,-5 0,0 3,-2 6,3 4,-1 7,-2 7,-6 4,-2 6,2 1,2-3,0-3,-1-4,4-3,0-5,4-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4149.15">3198 595,'0'3,"0"6,0 4,0 7,3 11,2 8,-1 8,4 6,3 5,0-3,2-4,2-4,2-6,-2-6,1-9,-4-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5178.76">3600 616,'-4'0,"1"0,-1 0,1 1,0-1,-1 1,1 0,0 0,0 0,-1 0,1 1,0-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1 1,1-1,0 1,0 0,0-1,0 1,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,0 5,-3 10,2 1,0 0,1-1,2 29,0-25,-1-12,1 0,0 0,0 0,1-1,0 1,1 0,0-1,1 0,0 1,0-2,1 1,0 0,1-1,0 0,0 0,0-1,1 1,14 10,-5-6,1-1,0-1,1 0,1-1,-1-1,1-1,0 0,27 4,-2 0,0-2,1-2,0-3,0-1,52-3,-94 0,0-1,0 0,0 1,0-1,0 0,0-1,0 1,0 0,0-1,-1 0,1 1,-1-1,1 0,-1 0,0 0,1-1,-1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 0,0 0,0 0,0 0,-1 0,1 0,0-6,1-9,-1-1,-1 1,-1-1,-2-19,1 20,0 7,0 1,0 0,-1-1,-1 1,0 1,0-1,-1 0,0 1,-1 0,0 0,0 1,-1-1,0 2,0-1,-1 1,0 0,-15-10,-2 0,0 2,-2 0,0 1,0 2,-30-9,31 14,0 1,0 1,-1 1,1 2,-1 0,-30 3,39 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6259.55">4616 384,'-33'-1,"20"0,0 0,1 2,-1-1,-24 5,37-5,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 0,0 1,-1-1,1 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,-1 1,1-1,0 0,0 1,12 4,25 0,148-4,-257-1,50 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7594.95">4976 108,'0'-2,"1"-1,0 1,-1 0,1 0,0 1,1-1,-1 0,0 0,0 0,1 1,-1-1,1 1,3-3,24-19,-12 13,1 0,34-14,-47 21,1 1,0 0,0 1,0-1,0 1,0 0,0 1,0-1,0 1,0 1,1-1,-1 1,10 2,-14-2,0 0,0 1,0-1,0 0,0 1,0-1,-1 1,1 0,0 0,-1-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,-1 0,1 1,-1-1,1 0,-1 1,0-1,0 0,0 1,0-1,-1 1,1-1,0 0,-1 0,-1 4,0 1,0 1,0 0,-1 0,0-1,-1 0,1 0,-1 0,-7 9,-33 21,44-37,0 1,0-1,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,-1 0,1 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,19 1,-17-1,56 0,108 7,-148-4,0 0,-1 1,0 1,0 0,0 2,31 15,-46-21,1 2,-1-1,1 0,-1 1,0-1,0 1,0 0,0 0,0 0,-1 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,-1 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0 0,0 0,-1 1,-1 6,-1-3,1 0,-1-1,0 1,-1-1,0 0,0 0,0 0,-1 0,0-1,0 1,-1-2,0 1,0 0,-7 4,-5 1,-1 0,1-2,-1 0,-1-1,0-1,0-1,0-1,-30 4,-6-3,-107-1,144-6</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink335.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:01:39.881"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'0'700,"0"-681</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">298 742,'3'0,"2"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink336.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:01:39.882"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2 786,'-1'-23,"0"8,1 1,1-1,0 0,4-18,-4 30,0 0,-1 0,1 0,0 1,1-1,-1 0,0 0,1 1,0-1,-1 1,1 0,0-1,0 1,0 0,1 0,-1 0,0 0,1 1,-1-1,1 1,0-1,-1 1,1 0,0 0,0 0,5 0,0-1,0 1,0 1,0-1,0 1,0 1,0-1,0 1,-1 1,1 0,0 0,13 5,-17-4,0-1,0 0,0 1,0 0,-1 0,1 1,-1-1,0 0,0 1,0 0,0 0,-1 0,1 0,-1 0,0 1,0-1,-1 0,1 1,-1 0,0-1,0 6,2 10,-1 0,-1 0,-1 1,-1-1,-1 0,-1 0,0 0,-2 0,0-1,-1 0,-1 0,0 0,-2-1,0 0,-1 0,-1-1,-1-1,-17 21,11-18,13-14,-1 1,1 0,0 0,0 1,1-1,-5 11,8-16,1-1,0 1,0 0,-1-1,1 1,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,0 1,1-1,-1 1,0 0,1-1,0 1,19 7,32-8,-44 0,104-4,-94 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">510 765,'-1'-20,"1"1,1-1,2 1,7-35,-9 49,0 1,1-1,0 1,0 0,0-1,0 1,1 0,-1 1,1-1,0 0,0 1,1 0,-1-1,1 1,0 1,-1-1,1 0,0 1,1 0,-1 0,0 0,0 0,1 1,-1 0,1 0,5-1,-3 1,0 0,1 1,-1 0,0 0,1 0,-1 1,10 2,-14-2,0 0,0 0,0 0,0 1,-1 0,1-1,-1 1,1 0,-1 0,1 0,-1 0,0 1,0-1,0 1,0-1,-1 1,1 0,-1-1,3 6,1 6,15 34,22 82,-38-115,-1-1,-1 1,0 0,-1 0,-1 0,0-1,-1 1,0 0,-2 0,-5 23,2-27,1 1,-2-1,0-1,0 1,-1-1,-14 15,7-7,-5-1,17-15,1-1,-1 1,1 0,0 0,-1 0,1 0,0 1,0-1,0 1,1-1,-1 1,0 0,1-1,0 1,0 0,-2 5,3-7,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0-1,-1 1,1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,0 0,0 0,0 0,2 0,44 2,-39-2,124-1,-107 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1378 638,'-52'-2,"34"0,-1 2,0 0,1 1,-36 6,52-6,-1 0,1 1,-1-1,1 0,0 1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 1,1-1,0 1,-1-1,1 1,0-1,0 1,1 0,-1 0,1-1,-1 1,1 0,0 0,0 5,0-4,0 0,0 0,0 0,1 0,0 0,-1-1,1 1,1 0,-1 0,0-1,1 1,0-1,0 1,0-1,0 0,1 1,-1-1,1 0,5 4,-1-3,0 0,1-1,-1 0,1-1,0 0,-1 0,1 0,15 1,69-3,-62-1,-24 1,0-1,1 1,-1-1,0 0,0-1,0 0,0 0,-1 0,1 0,-1-1,1 0,-1 0,0 0,0-1,0 0,5-5,-5 3,0 0,0 0,0-1,-1 0,0 0,0-1,-1 1,0-1,0 1,-1-1,3-14,-2 6,-2-1,0 1,-1-22,1 164,4 79,0-164,2-1,13 48,-11-64</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1928 743,'2'0,"0"1,0 0,1 0,-1 0,0 0,0 1,0-1,0 0,0 1,0-1,0 1,0 0,-1 0,3 3,2 2,11 9,196 191,-149-149,104 69,-118-92,2-3,0-2,97 39,-144-67,0 0,1-1,-1 1,1-1,-1-1,1 1,6-1,-10 0,-1 0,0 0,1 0,-1-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 0,1 0,0 0,0-1,-1 1,1 0,-1 0,1 0,-1-1,0 1,0 0,1 0,-1-1,0-1,0-15</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">2478 828,'-4'0,"-4"0,-5 0,0 3,-2 6,3 4,-1 7,-2 7,-6 4,-2 6,2 1,2-3,0-3,-1-4,4-3,0-5,4-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">3198 595,'0'3,"0"6,0 4,0 7,3 11,2 8,-1 8,4 6,3 5,0-3,2-4,2-4,2-6,-2-6,1-9,-4-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">3600 616,'-4'0,"1"0,-1 0,1 1,0-1,-1 1,1 0,0 0,0 0,-1 0,1 1,0-1,0 1,0 0,1 0,-1 0,0 0,1 0,-1 1,1-1,0 1,0 0,0-1,0 1,0 0,1 0,-1 0,1 0,0 1,0-1,0 0,0 5,-3 10,2 1,0 0,1-1,2 29,0-25,-1-12,1 0,0 0,0 0,1-1,0 1,1 0,0-1,1 0,0 1,0-2,1 1,0 0,1-1,0 0,0 0,0-1,1 1,14 10,-5-6,1-1,0-1,1 0,1-1,-1-1,1-1,0 0,27 4,-2 0,0-2,1-2,0-3,0-1,52-3,-94 0,0-1,0 0,0 1,0-1,0 0,0-1,0 1,0 0,0-1,-1 0,1 1,-1-1,1 0,-1 0,0 0,1-1,-1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,-1 0,0 0,0 0,0 0,-1 0,1 0,0-6,1-9,-1-1,-1 1,-1-1,-2-19,1 20,0 7,0 1,0 0,-1-1,-1 1,0 1,0-1,-1 0,0 1,-1 0,0 0,0 1,-1-1,0 2,0-1,-1 1,0 0,-15-10,-2 0,0 2,-2 0,0 1,0 2,-30-9,31 14,0 1,0 1,-1 1,1 2,-1 0,-30 3,39 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">4616 384,'-33'-1,"20"0,0 0,1 2,-1-1,-24 5,37-5,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,0 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 1,0-1,-1 0,1 0,0 1,-1-1,1 0,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,-1 1,1-1,0 0,0 1,12 4,25 0,148-4,-257-1,50 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">4976 108,'0'-2,"1"-1,0 1,-1 0,1 0,0 1,1-1,-1 0,0 0,0 0,1 1,-1-1,1 1,3-3,24-19,-12 13,1 0,34-14,-47 21,1 1,0 0,0 1,0-1,0 1,0 0,0 1,0-1,0 1,0 1,1-1,-1 1,10 2,-14-2,0 0,0 1,0-1,0 0,0 1,0-1,-1 1,1 0,0 0,-1-1,0 1,1 0,-1 0,0 0,0 1,0-1,0 0,0 0,-1 0,1 1,-1-1,1 0,-1 1,0-1,0 0,0 1,0-1,-1 1,1-1,0 0,-1 0,-1 4,0 1,0 1,0 0,-1 0,0-1,-1 0,1 0,-1 0,-7 9,-33 21,44-37,0 1,0-1,-1 0,1 0,0 0,0 0,0 0,0 1,0-1,-1 0,1 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,19 1,-17-1,56 0,108 7,-148-4,0 0,-1 1,0 1,0 0,0 2,31 15,-46-21,1 2,-1-1,1 0,-1 1,0-1,0 1,0 0,0 0,0 0,-1 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,-1 0,0 0,0 0,0 0,-1 0,1 0,-1 0,0 0,0 0,0 0,-1 1,-1 6,-1-3,1 0,-1-1,0 1,-1-1,0 0,0 0,0 0,-1 0,0-1,0 1,-1-2,0 1,0 0,-7 4,-5 1,-1 0,1-2,-1 0,-1-1,0-1,0-1,0-1,-30 4,-6-3,-107-1,144-6</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink337.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:02:27.344"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1505,'258'0,"-298"0,16 2,0-2,0-1,0-1,0 0,-44-12,68 14,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,-1-1,1 1,0 0,0 0,-1 0,1 0,0 0,0-1,-1 1,1 0,0 0,0 0,-1-1,1 1,0 0,0 0,0 0,0-1,0 1,-1 0,1-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0 0,0-1,0 1,1 0,-1 0,0-1,0 1,0 0,0 0,1-1,-1 1,8-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="600.33">1314 701,'0'1187,"-1"-1149,0-17,1 0,1-1,1 1,5 27,-7-47,0 0,1-1,-1 1,0 0,0 0,0 0,0-1,1 1,-1 0,0 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,0 1,-1-1,2 1,-2-1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,1 1,-1-1,0 1,1-1,-1 1,0-1,0 1,1-1,-1 0,0 0,10-38,-6 7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1246.83">1229 1378,'-50'-2,"0"-2,-64-13,-95-32,142 32,57 15,2 0,0 0,1 0,-1-1,1 0,-7-3,12 4,0 1,0 0,0-1,0 1,0-1,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,1-1,-1 1,0 0,1-1,-1-4,-1-46,6-77,0 32,-2-100,-2 165</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2567.44">1737 1781,'3'0,"5"0,5 0,4 0,-5 0,-4-4,-4-5,1-4,4 0,3 2,1 7,-7 4,-7 1,-8 2,-1-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3082.22">2054 680,'6'172,"7"-1,50 237,-46-304,-10-48,18 62,-24-116,0 1,-1-1,1 1,0-1,0 1,0-1,1 0,-1 0,1 0,-1 1,1-1,0 0,-1-1,1 1,0 0,4 2,-4-3,0-1,0 1,0-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,0-1,0 0,0 1,-1-1,1 0,0 0,2-2,9-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3650.97">2901 743,'0'3,"0"6,0 11,0 17,0 20,0 19,3 21,5 12,5 3,4-5,-1-12,0-19,-2-19,-4-23,-4-17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4619.04">2901 1188,'-66'0,"-91"12,147-10,3-1,0 0,0 0,0 0,0-1,-13-2,18 2,1 0,-1-1,0 1,1-1,-1 0,0 1,1-1,0 0,-1 0,1 0,-1 0,1 0,0-1,0 1,-1 0,1 0,0-1,0 1,1-1,-1 1,0-1,0 1,1-1,-1 0,1 1,-1-1,1 0,0 1,-1-3,-1-33,0 0,6-43,-2 17,-1 34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6040.44">3748 849,'-37'-1,"18"0,1 0,0 2,0 0,-29 6,42-6,1 0,1 0,-1 0,0 1,0 0,0 0,1 0,-1 0,1 0,-1 1,1 0,0-1,0 1,0 1,1-1,-1 0,1 0,0 1,0 0,0-1,0 1,0 0,1 0,0 0,-2 6,1 0,0 1,1 0,0 1,1-1,0 0,0 0,1 0,1 0,4 15,-5-23,1-1,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0-1,0 1,1-1,-1 0,1 1,-1-1,1 0,-1 0,1-1,0 1,-1 0,1-1,0 0,-1 0,1 0,0 0,0 0,-1 0,5-1,3-1,-1 1,0-1,0 0,-1-1,1 0,0-1,8-4,-11 4,0 0,0 0,0-1,0 0,-1 0,0 0,0-1,0 1,-1-1,0-1,0 1,-1 0,1-1,-1 0,-1 0,1 0,-1 0,0 0,1-11,3-4,-5 22,-1 0,0 0,1 0,-1 0,1 1,-1-1,0 0,0 0,1 1,-1-1,0 0,1 0,-1 1,0-1,0 0,0 1,1-1,-1 0,0 1,0-1,0 0,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 1,8 48,82 518,-82-524</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6929.19">4277 1061,'1'16,"2"1,1 0,0-1,0 0,2 0,0 0,1-1,13 22,-1 2,-17-35,77 155,-62-129,1-1,2-1,25 29,-39-50,0 0,1-1,-1 0,1 0,1 0,-1-1,1 0,0-1,9 5,-16-9,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1-1,1 1,-1 0,1 0,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,0-1,1 1,-1 0,0-1,1 1,-1-1,1 0,-1-1,0 1,1-1,-1 1,0-1,0 0,0 1,0-1,0 1,0-1,0 1,-2-4,-5-14</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7356.99">4340 997,'-1'3,"-2"10,-5 11,-5 14,-4 8,-2 9,2 7,0 7,3 3,0-4,-1-2,3-6,2-9,11-17,15-21,13-21,1-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7807.79">4891 934,'-1'3,"1"6,1 7,2 6,2 12,3 12,0 9,3 2,3 2,2 2,-1 2,-3-7,-4-6,-3-7,1-11,4-11,-1-10</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8868.43">5335 870,'-3'0,"0"0,0 0,0 0,0 1,0-1,0 1,1 0,-1 0,0 0,1 0,-1 1,0-1,1 0,0 1,-1 0,1 0,-2 2,0 0,1-1,1 1,-1 1,0-1,1 0,0 1,0-1,0 1,-1 6,-1 7,1 2,1-1,0 38,2-55,-1 34,0-1,1-1,2 0,1 0,13 61,-14-87,1 0,-1-1,1 0,1 1,-1-1,1 0,0-1,1 1,0-1,0 0,0 0,0 0,1 0,0-1,1 0,-1-1,1 1,0-1,0-1,0 1,0-1,0 0,1-1,0 0,-1 0,13 1,16 0,-1-1,66-7,-96 5,0 0,0-1,0 0,0 0,0-1,0 1,-1-1,1 0,0 0,-1 0,0-1,1 0,-1 1,0-2,0 1,-1 0,1-1,-1 1,0-1,0 0,0 0,0-1,-1 1,1-1,-1 1,0-1,-1 0,3-7,0-10,-1-1,0 1,-2-1,-1 0,-2-24,0 6,2 27,-1 1,-1 0,0-1,-1 1,-1 0,0 0,0 0,-2 1,1 0,-1 0,-1 0,0 0,-1 1,0 1,-1-1,0 1,-1 1,0 0,0 0,-1 1,0 0,0 1,-1 0,0 0,0 2,0 0,-1 0,0 1,0 0,0 1,0 1,-19-1,-15 2,28 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9683.52">5886 278,'-367'0,"404"0,-35 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10987.23">6161 3,'-46'-2,"23"1,0 1,-33 4,52-3,1 0,-1 0,1 0,-1 1,1-1,0 1,0 0,0 0,0 0,0 1,0-1,0 1,1-1,-1 1,1 0,0 0,0 0,0 0,0 0,1 1,-1-1,1 0,0 1,0-1,0 1,0 0,0 4,-1 8,0 0,1 0,1-1,1 1,2 17,-3-31,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,1-1,-1 1,1-1,-1 1,1-1,0 0,-1 0,1 0,0 0,0 0,-1 0,1-1,0 1,0 0,0-1,0 1,0-1,4 0,5 0,0 0,1-1,-1 0,21-6,-3 1,41 0,110 4,-112 2,-58 1,0 1,-1-1,1 1,0 1,0 0,-1 0,0 1,0 0,0 1,0 0,-1 0,15 13,-9-7,-1 1,0 0,-1 1,-1 1,0 0,13 22,-19-27,-1 1,0 0,-1 0,0 0,-1 1,0-1,-1 1,0-1,0 1,-1-1,-1 1,0 0,0-1,-1 1,-3 11,2-17,0 1,0-1,0 0,0-1,-1 1,0-1,0 1,0-1,0 0,-1 0,-6 3,-56 33,52-34,1 0,-1-1,0-1,-1-1,1 0,-1-1,1 0,-1-1,-23-2,22 0,0-1,0 0,0-2,0 0,1 0,-1-2,1 0,-23-12,22 6,4-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink338.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-06-05T21:03:12.365"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">409 130,'-10'-2,"1"0,0 0,0 0,0-2,0 1,0-1,1 0,0 0,-15-12,-7-2,9 7,-60-30,72 38,1 0,-1 0,1 1,-1 0,0 0,0 1,-17 0,24 1,-1 1,1-1,-1 1,1-1,0 1,-1 0,1 0,-1 0,1 0,0 0,0 0,0 1,0-1,0 1,0 0,-3 3,1-1,1 1,0 0,0 0,0 0,1 0,0 0,-2 7,-1 6,1 1,1-1,-2 28,4-26,-1 1,1 0,0 1,2-1,1 1,4 24,-5-43,0-1,-1 1,1-1,1 1,-1-1,0 1,1-1,-1 0,1 0,-1 1,1-1,0 0,0-1,0 1,0 0,1-1,-1 1,0-1,1 1,-1-1,1 0,-1 0,1 0,-1 0,1-1,0 1,-1-1,1 0,0 1,0-1,-1-1,1 1,0 0,-1 0,1-1,0 0,3-1,0 1,0-1,0 0,0-1,-1 0,1 1,-1-2,1 1,-1-1,0 1,0-1,-1-1,1 1,-1-1,0 1,6-10,-5 0,1 1,-2 0,6-25,9-29,-13 52,-5 12,0 0,0-1,0 1,1 0,-1 0,1 0,0 0,3-4,-4 7,-1-1,0 1,1 0,-1 0,1 0,-1-1,0 1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,16 19,14 35,-15-24,22 29,-15-25,-17-24,0 0,1 0,1-1,-1 0,15 12,-9-12</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -31163,7 +31529,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">219 0,'-1'1,"-1"-1,1 0,0 0,0 1,0-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 1,0 0,1 0,-1-1,0 1,1 0,-1 0,-1 1,-2 4,-21 24,2 0,2 1,0 2,3 0,-21 47,30-55,0-1,1 2,1-1,2 1,0 0,2 0,1 0,2 49,0-71,1-1,-1 1,1 0,0-1,0 1,0-1,1 1,-1-1,1 1,0-1,0 0,0 0,0 0,1 0,-1 0,1-1,-1 1,1-1,0 1,0-1,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,-1 0,1 0,-1-1,1 1,0-1,0 0,3 0,7 0,0 0,-1-1,1-1,0 0,-1-1,0-1,0 0,16-7,-17 6,0-1,-1 0,0-1,0 0,-1-1,0 0,0-1,-1 0,0 0,-1-1,0 0,0 0,7-14,-8 9,-1 1,0-2,-1 1,0 0,-1-1,-1 0,-1 0,0 0,-1 0,-1-19,0 21,0-5,-1 1,0-1,-2 1,0 0,-6-21,8 35,-1-1,0 1,0 0,0 0,-1 0,1 0,-1 0,0 0,0 1,-1-1,1 1,-1 0,1 0,-1 0,0 0,0 1,0 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,1 0,-6 0,-14-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.32">404 79,'4'0,"2"18,0 29,-1 24,-11 17,-4 13,-5 16,0-3,3-17,3-15,3-18,8-19,7-18,7-13,1-9</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.31">404 79,'4'0,"2"18,0 29,-1 24,-11 17,-4 13,-5 16,0-3,3-17,3-15,3-18,8-19,7-18,7-13,1-9</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1912.15">1171 211,'-5'0,"0"0,0-1,0 2,0-1,0 0,0 1,1 0,-1 0,0 1,1-1,-1 1,1 0,-1 0,1 1,0-1,0 1,0 0,0 0,0 0,1 0,-1 1,1 0,0-1,0 1,0 0,1 1,-1-1,-1 5,-12 24,2 1,1 0,1 1,3 0,0 1,2 0,-3 67,10-96,0 1,1 0,0-1,0 1,0-1,1 0,1 1,-1-1,1 0,0 0,1-1,0 1,0 0,0-1,1 0,0 0,0-1,0 1,1-1,-1 0,1-1,1 1,-1-1,1 0,-1-1,1 0,9 3,1 1,0-1,1-1,0-1,0 0,0-2,0 0,1-1,-1-1,0 0,25-5,-35 4,0 0,-1-1,1-1,-1 1,0-1,0 0,0-1,0 0,-1 0,1 0,-1-1,0 0,0 0,-1 0,1-1,-1 0,-1 0,1 0,-1-1,6-10,-4 3,-1 0,0-1,-1 1,-1-1,0 0,-1 0,0 0,-1 0,-2-27,1 33,0-1,-1 1,0 0,0-1,-1 1,0 0,-1 0,0 0,0 0,-1 1,0-1,-1 1,1 0,-11-13,0 6,1 1,-2 1,1 1,-2 0,0 1,0 0,-34-13,12 8</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3358.16">1753 344,'-12'28,"3"0,0 0,-5 34,1-10,6-26,1 0,2 0,0 0,2 0,1 48,2-69,0 0,1 0,-1-1,1 1,0 0,1-1,-1 1,1-1,0 0,0 0,0 0,0 0,1-1,0 1,-1-1,1 0,0 0,1 0,-1-1,7 4,13 6,0-2,43 13,-46-17,2 1,1-1,0-2,0 0,31 0,-39-3,0-1,-1-1,1-1,0 0,-1-1,0 0,24-9,-34 9,-1 0,1 0,-1 0,1-1,-1 1,0-1,0 0,-1 0,1-1,-1 1,0-1,0 0,0 0,-1 0,0 0,0 0,0 0,-1-1,1 1,-1 0,0-1,-1 1,0-1,0-10,0-7,-2-1,0 1,-2 0,-10-36,11 44,-1 0,-1 0,-1 1,0 0,-1 0,0 0,-1 0,-1 1,0 1,-1 0,0 0,-1 1,0 0,0 0,-2 2,1-1,-1 2,0-1,-1 2,0 0,-19-7,13 7,-1 0,-39-7,33 10</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4564.02">2918 79,'-4'74,"-3"-2,-24 104,-3 32,33-199,0-1,0 1,1 0,0-1,1 1,0 0,0-1,5 14,-5-19,0 0,1 0,-1 0,1-1,0 1,0 0,0-1,0 1,1-1,-1 0,1 0,-1 0,1 0,0 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,0 0,0-1,1 1,4-1,52 3,76-7,-41 1,-39 3,-22 1,1-2,-1-1,68-13,-49-2</inkml:trace>
@@ -31886,7 +32252,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">39 0,'4'131,"7"0,6-1,40 149,-1-23,-11 1,-12 2,-6 436,-29-661,0 0,-2 1,-1-2,-2 1,-2-1,-1 0,-2-1,-1 0,-2 0,-1-1,-2-1,-35 46,-47 43,78-92</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1242.1">1103 101,'-10'1,"2"1,0-1,1 2,-2-1,1 1,1 0,-1-1,1 2,-1 0,1 0,0 1,1 0,-1-1,0 1,2 1,-1 0,-5 6,-3 4,2-1,0 2,0 0,2 0,-14 31,22-45,1 1,-1 0,1 0,0 0,0 0,1-1,-1 1,1 0,0 1,0-1,0 0,0 0,1-1,0 1,-1 0,2 0,-1 0,0 0,1-1,0 0,0 1,0 0,0-1,6 6,1-1,0 0,1-1,1 0,-1-1,0 0,2 0,15 5,-12-5,0 2,1 0,-2-1,1 2,-1 1,0-1,-1 2,-1 0,1 1,-2-1,-1 2,1 0,-1 0,-2 1,1 0,-1 0,-1 1,-1 0,0 1,-1-1,0 0,3 33,-8-46,8 115,-7-101,-1-1,-1-1,-1 2,0-2,-8 25,9-36,-1 1,-1-2,2 1,-1 0,-1 0,1 0,0-1,-1 1,0 0,1-1,-1 0,0-1,0 1,0 0,-1 0,0 0,1-1,-1 0,1 0,-1 0,1 0,-8 1,-7 0,-2 0,2-1,-25-2,23 0,-199-8,194 8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1242.09">1103 101,'-10'1,"2"1,0-1,1 2,-2-1,1 1,1 0,-1-1,1 2,-1 0,1 0,0 1,1 0,-1-1,0 1,2 1,-1 0,-5 6,-3 4,2-1,0 2,0 0,2 0,-14 31,22-45,1 1,-1 0,1 0,0 0,0 0,1-1,-1 1,1 0,0 1,0-1,0 0,0 0,1-1,0 1,-1 0,2 0,-1 0,0 0,1-1,0 0,0 1,0 0,0-1,6 6,1-1,0 0,1-1,1 0,-1-1,0 0,2 0,15 5,-12-5,0 2,1 0,-2-1,1 2,-1 1,0-1,-1 2,-1 0,1 1,-2-1,-1 2,1 0,-1 0,-2 1,1 0,-1 0,-1 1,-1 0,0 1,-1-1,0 0,3 33,-8-46,8 115,-7-101,-1-1,-1-1,-1 2,0-2,-8 25,9-36,-1 1,-1-2,2 1,-1 0,-1 0,1 0,0-1,-1 1,0 0,1-1,-1 0,0-1,0 1,0 0,-1 0,0 0,1-1,-1 0,1 0,-1 0,1 0,-8 1,-7 0,-2 0,2-1,-25-2,23 0,-199-8,194 8</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1906.66">1429 1402,'4'0,"8"0,4 0,6 0,3 0,1 0,2 0,1 0,-1 0,5 0,10 0,13 0,5 0,2 0,-6 0,-11 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2559.84">1539 1835,'0'5,"4"1,7-2,6 1,4-2,4-1,2-1,5 0,25-1,93-1,60 1,19 0,3 0,-34 0,-51-1</inkml:trace>
 </inkml:ink>
@@ -31916,7 +32282,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">423 1064,'-10'0,"-1"0,1 0,0 1,0-1,-1 2,2-1,-1 2,0 0,1 0,-1 1,1 0,0-1,0 2,1 0,0 0,-1 1,1-1,0 2,1 0,0-1,1 1,-1 1,-6 10,-11 18,1 1,3 2,-26 66,38-81,0 0,2 0,1 1,1-2,0 2,3 0,2 45,0-67,-1-1,0 1,2-1,-2 0,1 0,-1 0,1 1,0-1,0 0,0 1,1-1,-1 0,0 0,1-1,0 1,-1 0,1-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1-1,2 1,-2-1,1 0,-1 0,1 0,-1 0,5-1,10-1,0-1,0-1,-2 0,29-11,-20 6,340-102,-352 107,1 0,-1-1,1-1,-2 0,1 0,13-11,-21 15,-1-2,2 1,-2-1,0 0,0 0,0 1,-1-1,1-1,-1 1,0-1,1 2,-2-2,1 0,-1 0,0 0,0 1,-1 0,1-1,-1-5,-1-6,1 2,-2-1,0-1,-1 2,-2 0,-4-16,6 23,-1 1,0-2,0 1,0 1,0 0,-1 0,0-1,-1 2,0 0,1-1,-1 1,-2 1,-9-7,-12-3</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="569.81">1197 1569,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="569.8">1197 1569,'0'0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1451.34">1695 710,'0'1,"1"-1,0 1,0 0,0-1,-1 1,1-1,0 0,-1 1,1 0,-1 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 1,4 28,-3-24,6 89,-5 0,-19 152,9-146,-2-43,7-44,1 2,0-1,1 0,2 29,-1-42,1 0,-1 0,1-1,-1 1,1 0,0 0,0-1,0 1,0-1,0 0,0 1,1-1,0 0,-1 1,1-1,-1 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0-1,0 1,0 0,-1-1,4 1,58 2,-49-3,19 0,22 0,-2 0,76-12,-100 5</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2039.62">2110 633,'13'208,"-1"-86,67 580,-75-666,-1-9</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3010.93">174 481,'-2'14,"0"0,-1-2,-1 2,0-1,0-1,-2 1,-9 17,-17 40,-4 109,-1-4,27-122,1-1,3 1,3 1,7 96,-1-31,-3-83,1-1,2-1,11 40,-10-57,1 0,2 0,-1-1,1-1,2 1,0-1,0 0,18 19,1-2,64 56,-81-78,1-1,0 0,2 0,-1-2,1 1,0-1,0-2,1 1,16 4,0-5</inkml:trace>
@@ -33551,7 +33917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E85375-9F39-4F09-B741-414DFA1AB951}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="P66" sqref="P66"/>
     </sheetView>
   </sheetViews>
@@ -33566,8 +33932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517F12C5-8AB8-4800-9E76-979D7AAD4624}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>